<commit_message>
submit capstone 1 - 05 modeling
</commit_message>
<xml_diff>
--- a/models/regression_model_1m/pycaret_tables.xlsx
+++ b/models/regression_model_1m/pycaret_tables.xlsx
@@ -586,7 +586,7 @@
         <v>0.0847</v>
       </c>
       <c r="I2">
-        <v>0.046</v>
+        <v>0.058</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -615,7 +615,7 @@
         <v>0.08450000000000001</v>
       </c>
       <c r="I3">
-        <v>0.07199999999999999</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -644,7 +644,7 @@
         <v>0.0914</v>
       </c>
       <c r="I4">
-        <v>0.03</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -673,7 +673,7 @@
         <v>0.0892</v>
       </c>
       <c r="I5">
-        <v>0.08799999999999999</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -702,7 +702,7 @@
         <v>0.1033</v>
       </c>
       <c r="I6">
-        <v>0.042</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -731,7 +731,7 @@
         <v>0.1191</v>
       </c>
       <c r="I7">
-        <v>1.11</v>
+        <v>1.028</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -789,7 +789,7 @@
         <v>0.1208</v>
       </c>
       <c r="I9">
-        <v>0.02</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -818,7 +818,7 @@
         <v>0.1244</v>
       </c>
       <c r="I10">
-        <v>0.024</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -847,7 +847,7 @@
         <v>0.1226</v>
       </c>
       <c r="I11">
-        <v>0.51</v>
+        <v>0.534</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -876,7 +876,7 @@
         <v>0.106</v>
       </c>
       <c r="I12">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -934,7 +934,7 @@
         <v>0.1107</v>
       </c>
       <c r="I14">
-        <v>0.018</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -992,7 +992,7 @@
         <v>0.1519</v>
       </c>
       <c r="I16">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1021,7 +1021,7 @@
         <v>0.2712</v>
       </c>
       <c r="I17">
-        <v>0.018</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1050,7 +1050,7 @@
         <v>0.5058</v>
       </c>
       <c r="I18">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1188,22 +1188,22 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>2.6303</v>
+        <v>1.5421</v>
       </c>
       <c r="D2">
-        <v>10.763</v>
+        <v>3.8317</v>
       </c>
       <c r="E2">
-        <v>3.2807</v>
+        <v>1.9575</v>
       </c>
       <c r="F2">
-        <v>0.9781</v>
+        <v>0.9943</v>
       </c>
       <c r="G2">
-        <v>0.0521</v>
+        <v>0.0384</v>
       </c>
       <c r="H2">
-        <v>0.0437</v>
+        <v>0.0278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated datasets with November data
</commit_message>
<xml_diff>
--- a/models/regression_model_1m/pycaret_tables.xlsx
+++ b/models/regression_model_1m/pycaret_tables.xlsx
@@ -50,22 +50,25 @@
     <t>TT (Sec)</t>
   </si>
   <si>
+    <t>et</t>
+  </si>
+  <si>
     <t>gbr</t>
   </si>
   <si>
-    <t>et</t>
-  </si>
-  <si>
     <t>lightgbm</t>
   </si>
   <si>
     <t>rf</t>
   </si>
   <si>
+    <t>lr</t>
+  </si>
+  <si>
     <t>ada</t>
   </si>
   <si>
-    <t>lr</t>
+    <t>huber</t>
   </si>
   <si>
     <t>ridge</t>
@@ -74,9 +77,6 @@
     <t>br</t>
   </si>
   <si>
-    <t>huber</t>
-  </si>
-  <si>
     <t>lasso</t>
   </si>
   <si>
@@ -86,12 +86,12 @@
     <t>omp</t>
   </si>
   <si>
+    <t>en</t>
+  </si>
+  <si>
     <t>dt</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
     <t>par</t>
   </si>
   <si>
@@ -104,22 +104,25 @@
     <t>lar</t>
   </si>
   <si>
+    <t>Extra Trees Regressor</t>
+  </si>
+  <si>
     <t>Gradient Boosting Regressor</t>
   </si>
   <si>
-    <t>Extra Trees Regressor</t>
-  </si>
-  <si>
     <t>Light Gradient Boosting Machine</t>
   </si>
   <si>
     <t>Random Forest Regressor</t>
   </si>
   <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
     <t>AdaBoost Regressor</t>
   </si>
   <si>
-    <t>Linear Regression</t>
+    <t>Huber Regressor</t>
   </si>
   <si>
     <t>Ridge Regression</t>
@@ -128,9 +131,6 @@
     <t>Bayesian Ridge</t>
   </si>
   <si>
-    <t>Huber Regressor</t>
-  </si>
-  <si>
     <t>Lasso Regression</t>
   </si>
   <si>
@@ -140,10 +140,10 @@
     <t>Orthogonal Matching Pursuit</t>
   </si>
   <si>
+    <t>Elastic Net</t>
+  </si>
+  <si>
     <t>Decision Tree Regressor</t>
-  </si>
-  <si>
-    <t>Elastic Net</t>
   </si>
   <si>
     <t>Passive Aggressive Regressor</t>
@@ -568,25 +568,25 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>4.6119</v>
+        <v>4.5075</v>
       </c>
       <c r="D2">
-        <v>42.6163</v>
+        <v>40.471</v>
       </c>
       <c r="E2">
-        <v>6.3519</v>
+        <v>6.315</v>
       </c>
       <c r="F2">
-        <v>0.9407</v>
+        <v>0.946</v>
       </c>
       <c r="G2">
-        <v>0.1131</v>
+        <v>0.115</v>
       </c>
       <c r="H2">
-        <v>0.0847</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="I2">
-        <v>0.058</v>
+        <v>0.068</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -597,25 +597,25 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>4.4981</v>
+        <v>5.1025</v>
       </c>
       <c r="D3">
-        <v>44.6487</v>
+        <v>48.2418</v>
       </c>
       <c r="E3">
-        <v>6.458</v>
+        <v>6.8486</v>
       </c>
       <c r="F3">
-        <v>0.9384</v>
+        <v>0.9354</v>
       </c>
       <c r="G3">
-        <v>0.1131</v>
+        <v>0.1201</v>
       </c>
       <c r="H3">
-        <v>0.08450000000000001</v>
+        <v>0.0924</v>
       </c>
       <c r="I3">
-        <v>0.074</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -626,22 +626,22 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <v>4.8927</v>
+        <v>5.2173</v>
       </c>
       <c r="D4">
-        <v>45.0184</v>
+        <v>53.3653</v>
       </c>
       <c r="E4">
-        <v>6.5788</v>
+        <v>7.2457</v>
       </c>
       <c r="F4">
-        <v>0.9377</v>
+        <v>0.9288999999999999</v>
       </c>
       <c r="G4">
-        <v>0.1174</v>
+        <v>0.1223</v>
       </c>
       <c r="H4">
-        <v>0.0914</v>
+        <v>0.09329999999999999</v>
       </c>
       <c r="I4">
         <v>0.032</v>
@@ -655,22 +655,22 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>4.8434</v>
+        <v>5.2954</v>
       </c>
       <c r="D5">
-        <v>46.3525</v>
+        <v>55.0556</v>
       </c>
       <c r="E5">
-        <v>6.6849</v>
+        <v>7.3763</v>
       </c>
       <c r="F5">
-        <v>0.9361</v>
+        <v>0.9261</v>
       </c>
       <c r="G5">
-        <v>0.1174</v>
+        <v>0.1299</v>
       </c>
       <c r="H5">
-        <v>0.0892</v>
+        <v>0.09619999999999999</v>
       </c>
       <c r="I5">
         <v>0.092</v>
@@ -684,25 +684,25 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>5.4859</v>
+        <v>5.8957</v>
       </c>
       <c r="D6">
-        <v>52.53</v>
+        <v>56.6823</v>
       </c>
       <c r="E6">
-        <v>7.1626</v>
+        <v>7.4881</v>
       </c>
       <c r="F6">
-        <v>0.9276</v>
+        <v>0.9252</v>
       </c>
       <c r="G6">
-        <v>0.1289</v>
+        <v>0.1551</v>
       </c>
       <c r="H6">
-        <v>0.1033</v>
+        <v>0.118</v>
       </c>
       <c r="I6">
-        <v>0.046</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -713,25 +713,25 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>5.8856</v>
+        <v>5.7991</v>
       </c>
       <c r="D7">
-        <v>58.3605</v>
+        <v>59.5745</v>
       </c>
       <c r="E7">
-        <v>7.5929</v>
+        <v>7.6263</v>
       </c>
       <c r="F7">
         <v>0.9205</v>
       </c>
       <c r="G7">
-        <v>0.1659</v>
+        <v>0.1333</v>
       </c>
       <c r="H7">
-        <v>0.1191</v>
+        <v>0.1076</v>
       </c>
       <c r="I7">
-        <v>1.028</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -742,25 +742,25 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>5.9879</v>
+        <v>5.8054</v>
       </c>
       <c r="D8">
-        <v>58.5232</v>
+        <v>58.8903</v>
       </c>
       <c r="E8">
-        <v>7.6147</v>
+        <v>7.6361</v>
       </c>
       <c r="F8">
-        <v>0.9204</v>
+        <v>0.9222</v>
       </c>
       <c r="G8">
-        <v>0.163</v>
+        <v>0.1569</v>
       </c>
       <c r="H8">
-        <v>0.1188</v>
+        <v>0.1162</v>
       </c>
       <c r="I8">
-        <v>0.018</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -771,22 +771,22 @@
         <v>33</v>
       </c>
       <c r="C9">
-        <v>6.0679</v>
+        <v>5.9442</v>
       </c>
       <c r="D9">
-        <v>60.2652</v>
+        <v>59.6758</v>
       </c>
       <c r="E9">
-        <v>7.726</v>
+        <v>7.6896</v>
       </c>
       <c r="F9">
-        <v>0.9182</v>
+        <v>0.9207</v>
       </c>
       <c r="G9">
-        <v>0.1671</v>
+        <v>0.155</v>
       </c>
       <c r="H9">
-        <v>0.1208</v>
+        <v>0.1166</v>
       </c>
       <c r="I9">
         <v>0.018</v>
@@ -800,25 +800,25 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>6.2296</v>
+        <v>6.0204</v>
       </c>
       <c r="D10">
-        <v>65.2736</v>
+        <v>62.5989</v>
       </c>
       <c r="E10">
-        <v>8.0244</v>
+        <v>7.8761</v>
       </c>
       <c r="F10">
-        <v>0.9112</v>
+        <v>0.9165</v>
       </c>
       <c r="G10">
-        <v>0.1705</v>
+        <v>0.1584</v>
       </c>
       <c r="H10">
-        <v>0.1244</v>
+        <v>0.1173</v>
       </c>
       <c r="I10">
-        <v>0.026</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -829,25 +829,25 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>6.2749</v>
+        <v>6.2585</v>
       </c>
       <c r="D11">
-        <v>68.5926</v>
+        <v>68.0508</v>
       </c>
       <c r="E11">
-        <v>8.209300000000001</v>
+        <v>8.217499999999999</v>
       </c>
       <c r="F11">
-        <v>0.9074</v>
+        <v>0.9094</v>
       </c>
       <c r="G11">
-        <v>0.1594</v>
+        <v>0.1603</v>
       </c>
       <c r="H11">
-        <v>0.1226</v>
+        <v>0.1227</v>
       </c>
       <c r="I11">
-        <v>0.534</v>
+        <v>0.602</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -858,25 +858,25 @@
         <v>36</v>
       </c>
       <c r="C12">
-        <v>5.8394</v>
+        <v>5.8895</v>
       </c>
       <c r="D12">
-        <v>76.0692</v>
+        <v>73.73650000000001</v>
       </c>
       <c r="E12">
-        <v>8.6463</v>
+        <v>8.423999999999999</v>
       </c>
       <c r="F12">
-        <v>0.8983</v>
+        <v>0.9046999999999999</v>
       </c>
       <c r="G12">
-        <v>0.1417</v>
+        <v>0.1415</v>
       </c>
       <c r="H12">
-        <v>0.106</v>
+        <v>0.1092</v>
       </c>
       <c r="I12">
-        <v>0.02</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -887,25 +887,25 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>6.5508</v>
+        <v>6.3058</v>
       </c>
       <c r="D13">
-        <v>78.0218</v>
+        <v>75.9007</v>
       </c>
       <c r="E13">
-        <v>8.751099999999999</v>
+        <v>8.695600000000001</v>
       </c>
       <c r="F13">
-        <v>0.8944</v>
+        <v>0.8972</v>
       </c>
       <c r="G13">
-        <v>0.174</v>
+        <v>0.1697</v>
       </c>
       <c r="H13">
-        <v>0.1275</v>
+        <v>0.1241</v>
       </c>
       <c r="I13">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -916,25 +916,25 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>6.3379</v>
+        <v>6.8563</v>
       </c>
       <c r="D14">
-        <v>82.4756</v>
+        <v>79.071</v>
       </c>
       <c r="E14">
-        <v>8.9153</v>
+        <v>8.8599</v>
       </c>
       <c r="F14">
-        <v>0.8858</v>
+        <v>0.8949</v>
       </c>
       <c r="G14">
-        <v>0.1484</v>
+        <v>0.1657</v>
       </c>
       <c r="H14">
-        <v>0.1107</v>
+        <v>0.1325</v>
       </c>
       <c r="I14">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -945,25 +945,25 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>6.9746</v>
+        <v>6.6427</v>
       </c>
       <c r="D15">
-        <v>82.6238</v>
+        <v>84.36839999999999</v>
       </c>
       <c r="E15">
-        <v>9.057399999999999</v>
+        <v>9.0702</v>
       </c>
       <c r="F15">
-        <v>0.8883</v>
+        <v>0.8842</v>
       </c>
       <c r="G15">
-        <v>0.1659</v>
+        <v>0.1536</v>
       </c>
       <c r="H15">
-        <v>0.1332</v>
+        <v>0.1183</v>
       </c>
       <c r="I15">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -974,25 +974,25 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>7.4808</v>
+        <v>8.6614</v>
       </c>
       <c r="D16">
-        <v>94.4228</v>
+        <v>132.6311</v>
       </c>
       <c r="E16">
-        <v>9.523</v>
+        <v>10.8966</v>
       </c>
       <c r="F16">
-        <v>0.8731</v>
+        <v>0.8177</v>
       </c>
       <c r="G16">
-        <v>0.2444</v>
+        <v>0.3149</v>
       </c>
       <c r="H16">
-        <v>0.1519</v>
+        <v>0.1884</v>
       </c>
       <c r="I16">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1003,25 +1003,25 @@
         <v>41</v>
       </c>
       <c r="C17">
-        <v>13.0727</v>
+        <v>12.8847</v>
       </c>
       <c r="D17">
-        <v>245.198</v>
+        <v>249.6969</v>
       </c>
       <c r="E17">
-        <v>15.6182</v>
+        <v>15.7637</v>
       </c>
       <c r="F17">
-        <v>0.6698</v>
+        <v>0.6677</v>
       </c>
       <c r="G17">
-        <v>0.2858</v>
+        <v>0.2795</v>
       </c>
       <c r="H17">
-        <v>0.2712</v>
+        <v>0.2643</v>
       </c>
       <c r="I17">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1032,25 +1032,25 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>23.5358</v>
+        <v>23.2068</v>
       </c>
       <c r="D18">
-        <v>751.4456</v>
+        <v>756.9346</v>
       </c>
       <c r="E18">
-        <v>27.3783</v>
+        <v>27.4508</v>
       </c>
       <c r="F18">
-        <v>-0.008999999999999999</v>
+        <v>-0.0056</v>
       </c>
       <c r="G18">
-        <v>0.4839</v>
+        <v>0.4782</v>
       </c>
       <c r="H18">
-        <v>0.5058</v>
+        <v>0.4956</v>
       </c>
       <c r="I18">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1061,22 +1061,22 @@
         <v>43</v>
       </c>
       <c r="C19">
-        <v>111.3592</v>
+        <v>4382.0176</v>
       </c>
       <c r="D19">
-        <v>55904.4646</v>
+        <v>192874824.186</v>
       </c>
       <c r="E19">
-        <v>153.1446</v>
+        <v>6358.1619</v>
       </c>
       <c r="F19">
-        <v>-76.3618</v>
+        <v>-272295.7716</v>
       </c>
       <c r="G19">
-        <v>1.0019</v>
+        <v>1.8959</v>
       </c>
       <c r="H19">
-        <v>1.9531</v>
+        <v>75.4915</v>
       </c>
       <c r="I19">
         <v>0.02</v>
@@ -1126,22 +1126,22 @@
         <v>48</v>
       </c>
       <c r="C2">
-        <v>4.9824</v>
+        <v>5.2775</v>
       </c>
       <c r="D2">
-        <v>36.2245</v>
+        <v>44.2081</v>
       </c>
       <c r="E2">
-        <v>6.0187</v>
+        <v>6.6489</v>
       </c>
       <c r="F2">
-        <v>0.9263</v>
+        <v>0.9107</v>
       </c>
       <c r="G2">
-        <v>0.098</v>
+        <v>0.1042</v>
       </c>
       <c r="H2">
-        <v>0.0825</v>
+        <v>0.0881</v>
       </c>
     </row>
   </sheetData>
@@ -1185,25 +1185,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2">
-        <v>1.5421</v>
+        <v>0.9828</v>
       </c>
       <c r="D2">
-        <v>3.8317</v>
+        <v>1.9863</v>
       </c>
       <c r="E2">
-        <v>1.9575</v>
+        <v>1.4094</v>
       </c>
       <c r="F2">
-        <v>0.9943</v>
+        <v>0.9971</v>
       </c>
       <c r="G2">
-        <v>0.0384</v>
+        <v>0.0246</v>
       </c>
       <c r="H2">
-        <v>0.0278</v>
+        <v>0.0164</v>
       </c>
     </row>
   </sheetData>
@@ -1247,22 +1247,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.7133</v>
+        <v>4.4767</v>
       </c>
       <c r="C2">
-        <v>24.4168</v>
+        <v>35.6244</v>
       </c>
       <c r="D2">
-        <v>4.9413</v>
+        <v>5.9686</v>
       </c>
       <c r="E2">
-        <v>0.9664</v>
+        <v>0.9567</v>
       </c>
       <c r="F2">
-        <v>0.0733</v>
+        <v>0.0804</v>
       </c>
       <c r="G2">
-        <v>0.0585</v>
+        <v>0.06759999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1270,22 +1270,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.9891</v>
+        <v>3.6016</v>
       </c>
       <c r="C3">
-        <v>29.7275</v>
+        <v>36.6182</v>
       </c>
       <c r="D3">
-        <v>5.4523</v>
+        <v>6.0513</v>
       </c>
       <c r="E3">
-        <v>0.9636</v>
+        <v>0.9483</v>
       </c>
       <c r="F3">
-        <v>0.078</v>
+        <v>0.08890000000000001</v>
       </c>
       <c r="G3">
-        <v>0.0654</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1293,22 +1293,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2799</v>
+        <v>4.3482</v>
       </c>
       <c r="C4">
-        <v>35.5947</v>
+        <v>31.7973</v>
       </c>
       <c r="D4">
-        <v>5.9661</v>
+        <v>5.6389</v>
       </c>
       <c r="E4">
-        <v>0.9435</v>
+        <v>0.952</v>
       </c>
       <c r="F4">
-        <v>0.09370000000000001</v>
+        <v>0.0844</v>
       </c>
       <c r="G4">
-        <v>0.0706</v>
+        <v>0.0722</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1316,22 +1316,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.4232</v>
+        <v>6.447</v>
       </c>
       <c r="C5">
-        <v>17.9163</v>
+        <v>80.9879</v>
       </c>
       <c r="D5">
-        <v>4.2328</v>
+        <v>8.9993</v>
       </c>
       <c r="E5">
-        <v>0.9782999999999999</v>
+        <v>0.9112</v>
       </c>
       <c r="F5">
-        <v>0.0775</v>
+        <v>0.2168</v>
       </c>
       <c r="G5">
-        <v>0.0639</v>
+        <v>0.1636</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1339,22 +1339,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5.8833</v>
+        <v>4.2917</v>
       </c>
       <c r="C6">
-        <v>69.8308</v>
+        <v>38.2074</v>
       </c>
       <c r="D6">
-        <v>8.3565</v>
+        <v>6.1812</v>
       </c>
       <c r="E6">
-        <v>0.9035</v>
+        <v>0.9419</v>
       </c>
       <c r="F6">
-        <v>0.1901</v>
+        <v>0.115</v>
       </c>
       <c r="G6">
-        <v>0.1336</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1362,22 +1362,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.2578</v>
+        <v>4.633</v>
       </c>
       <c r="C7">
-        <v>35.4972</v>
+        <v>44.647</v>
       </c>
       <c r="D7">
-        <v>5.7898</v>
+        <v>6.5679</v>
       </c>
       <c r="E7">
-        <v>0.9510999999999999</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F7">
-        <v>0.1025</v>
+        <v>0.1171</v>
       </c>
       <c r="G7">
-        <v>0.0784</v>
+        <v>0.08890000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1385,22 +1385,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.8612</v>
+        <v>0.9567</v>
       </c>
       <c r="C8">
-        <v>18.1326</v>
+        <v>18.2927</v>
       </c>
       <c r="D8">
-        <v>1.4055</v>
+        <v>1.2289</v>
       </c>
       <c r="E8">
-        <v>0.0263</v>
+        <v>0.0162</v>
       </c>
       <c r="F8">
-        <v>0.0443</v>
+        <v>0.0513</v>
       </c>
       <c r="G8">
-        <v>0.0279</v>
+        <v>0.038</v>
       </c>
     </row>
   </sheetData>
@@ -1444,22 +1444,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.2013</v>
+        <v>4.6779</v>
       </c>
       <c r="C2">
-        <v>34.5914</v>
+        <v>34.3328</v>
       </c>
       <c r="D2">
-        <v>5.8814</v>
+        <v>5.8594</v>
       </c>
       <c r="E2">
-        <v>0.9524</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="F2">
-        <v>0.09089999999999999</v>
+        <v>0.0887</v>
       </c>
       <c r="G2">
-        <v>0.0673</v>
+        <v>0.0733</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1467,22 +1467,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.1276</v>
+        <v>5.3189</v>
       </c>
       <c r="C3">
-        <v>33.1818</v>
+        <v>59.4736</v>
       </c>
       <c r="D3">
-        <v>5.7604</v>
+        <v>7.7119</v>
       </c>
       <c r="E3">
-        <v>0.9594</v>
+        <v>0.916</v>
       </c>
       <c r="F3">
-        <v>0.0922</v>
+        <v>0.1146</v>
       </c>
       <c r="G3">
-        <v>0.07240000000000001</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1490,22 +1490,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.9935</v>
+        <v>3.875</v>
       </c>
       <c r="C4">
-        <v>34.371</v>
+        <v>23.571</v>
       </c>
       <c r="D4">
-        <v>5.8627</v>
+        <v>4.855</v>
       </c>
       <c r="E4">
-        <v>0.9454</v>
+        <v>0.9644</v>
       </c>
       <c r="F4">
-        <v>0.0907</v>
+        <v>0.0919</v>
       </c>
       <c r="G4">
-        <v>0.0665</v>
+        <v>0.0699</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1513,22 +1513,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.9575</v>
+        <v>5.5547</v>
       </c>
       <c r="C5">
-        <v>23.6778</v>
+        <v>57.3705</v>
       </c>
       <c r="D5">
-        <v>4.866</v>
+        <v>7.5743</v>
       </c>
       <c r="E5">
-        <v>0.9713000000000001</v>
+        <v>0.9371</v>
       </c>
       <c r="F5">
-        <v>0.0883</v>
+        <v>0.188</v>
       </c>
       <c r="G5">
-        <v>0.074</v>
+        <v>0.1366</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1536,22 +1536,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.3447</v>
+        <v>3.3128</v>
       </c>
       <c r="C6">
-        <v>91</v>
+        <v>20.7651</v>
       </c>
       <c r="D6">
-        <v>9.539400000000001</v>
+        <v>4.5569</v>
       </c>
       <c r="E6">
-        <v>0.8743</v>
+        <v>0.9684</v>
       </c>
       <c r="F6">
-        <v>0.1946</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="G6">
-        <v>0.1417</v>
+        <v>0.0626</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1559,22 +1559,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5249</v>
+        <v>4.5479</v>
       </c>
       <c r="C7">
-        <v>43.3644</v>
+        <v>39.1026</v>
       </c>
       <c r="D7">
-        <v>6.382</v>
+        <v>6.1115</v>
       </c>
       <c r="E7">
-        <v>0.9406</v>
+        <v>0.9488</v>
       </c>
       <c r="F7">
-        <v>0.1113</v>
+        <v>0.1143</v>
       </c>
       <c r="G7">
-        <v>0.0844</v>
+        <v>0.0863</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1582,22 +1582,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.9142</v>
+        <v>0.8489</v>
       </c>
       <c r="C8">
-        <v>24.1588</v>
+        <v>16.4252</v>
       </c>
       <c r="D8">
-        <v>1.6232</v>
+        <v>1.3237</v>
       </c>
       <c r="E8">
-        <v>0.0342</v>
+        <v>0.0196</v>
       </c>
       <c r="F8">
-        <v>0.0417</v>
+        <v>0.0381</v>
       </c>
       <c r="G8">
-        <v>0.0288</v>
+        <v>0.0266</v>
       </c>
     </row>
   </sheetData>
@@ -1641,22 +1641,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.6571</v>
+        <v>5.0395</v>
       </c>
       <c r="C2">
-        <v>33.542</v>
+        <v>45.9624</v>
       </c>
       <c r="D2">
-        <v>5.7915</v>
+        <v>6.7796</v>
       </c>
       <c r="E2">
-        <v>0.9539</v>
+        <v>0.9441000000000001</v>
       </c>
       <c r="F2">
-        <v>0.1039</v>
+        <v>0.0968</v>
       </c>
       <c r="G2">
-        <v>0.08119999999999999</v>
+        <v>0.0765</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1664,22 +1664,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.9068</v>
+        <v>5.2368</v>
       </c>
       <c r="C3">
-        <v>24.7167</v>
+        <v>63.5893</v>
       </c>
       <c r="D3">
-        <v>4.9716</v>
+        <v>7.9743</v>
       </c>
       <c r="E3">
-        <v>0.9698</v>
+        <v>0.9102</v>
       </c>
       <c r="F3">
-        <v>0.0837</v>
+        <v>0.1152</v>
       </c>
       <c r="G3">
-        <v>0.0699</v>
+        <v>0.0867</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1687,22 +1687,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.6063</v>
+        <v>4.6568</v>
       </c>
       <c r="C4">
-        <v>34.9543</v>
+        <v>32.5161</v>
       </c>
       <c r="D4">
-        <v>5.9122</v>
+        <v>5.7023</v>
       </c>
       <c r="E4">
-        <v>0.9445</v>
+        <v>0.9509</v>
       </c>
       <c r="F4">
-        <v>0.1003</v>
+        <v>0.1029</v>
       </c>
       <c r="G4">
-        <v>0.0809</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1710,22 +1710,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.9057</v>
+        <v>5.6617</v>
       </c>
       <c r="C5">
-        <v>22.8745</v>
+        <v>57.0659</v>
       </c>
       <c r="D5">
-        <v>4.7827</v>
+        <v>7.5542</v>
       </c>
       <c r="E5">
-        <v>0.9723000000000001</v>
+        <v>0.9374</v>
       </c>
       <c r="F5">
-        <v>0.08690000000000001</v>
+        <v>0.1773</v>
       </c>
       <c r="G5">
-        <v>0.07240000000000001</v>
+        <v>0.134</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1733,22 +1733,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.7308</v>
+        <v>5.0891</v>
       </c>
       <c r="C6">
-        <v>78.815</v>
+        <v>46.3525</v>
       </c>
       <c r="D6">
-        <v>8.877800000000001</v>
+        <v>6.8083</v>
       </c>
       <c r="E6">
-        <v>0.8911</v>
+        <v>0.9295</v>
       </c>
       <c r="F6">
-        <v>0.1909</v>
+        <v>0.1196</v>
       </c>
       <c r="G6">
-        <v>0.1469</v>
+        <v>0.0911</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1756,22 +1756,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.7613</v>
+        <v>5.1368</v>
       </c>
       <c r="C7">
-        <v>38.9805</v>
+        <v>49.0972</v>
       </c>
       <c r="D7">
-        <v>6.0672</v>
+        <v>6.9637</v>
       </c>
       <c r="E7">
-        <v>0.9463</v>
+        <v>0.9344</v>
       </c>
       <c r="F7">
-        <v>0.1131</v>
+        <v>0.1224</v>
       </c>
       <c r="G7">
-        <v>0.09030000000000001</v>
+        <v>0.0935</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1779,22 +1779,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>1.0369</v>
+        <v>0.3248</v>
       </c>
       <c r="C8">
-        <v>20.4716</v>
+        <v>10.6378</v>
       </c>
       <c r="D8">
-        <v>1.4731</v>
+        <v>0.7771</v>
       </c>
       <c r="E8">
-        <v>0.0294</v>
+        <v>0.014</v>
       </c>
       <c r="F8">
-        <v>0.0396</v>
+        <v>0.0287</v>
       </c>
       <c r="G8">
-        <v>0.0287</v>
+        <v>0.0209</v>
       </c>
     </row>
   </sheetData>
@@ -1838,22 +1838,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.1175</v>
+        <v>4.8397</v>
       </c>
       <c r="C2">
-        <v>33.9625</v>
+        <v>41.2268</v>
       </c>
       <c r="D2">
-        <v>5.8277</v>
+        <v>6.4208</v>
       </c>
       <c r="E2">
-        <v>0.9533</v>
+        <v>0.9498</v>
       </c>
       <c r="F2">
-        <v>0.08699999999999999</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="G2">
-        <v>0.067</v>
+        <v>0.07290000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1861,22 +1861,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.4045</v>
+        <v>4.7935</v>
       </c>
       <c r="C3">
-        <v>39.9219</v>
+        <v>52.8236</v>
       </c>
       <c r="D3">
-        <v>6.3184</v>
+        <v>7.268</v>
       </c>
       <c r="E3">
-        <v>0.9512</v>
+        <v>0.9254</v>
       </c>
       <c r="F3">
-        <v>0.09429999999999999</v>
+        <v>0.1071</v>
       </c>
       <c r="G3">
-        <v>0.0737</v>
+        <v>0.0774</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1884,22 +1884,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.6193</v>
+        <v>4.2358</v>
       </c>
       <c r="C4">
-        <v>39.3926</v>
+        <v>27.6849</v>
       </c>
       <c r="D4">
-        <v>6.2764</v>
+        <v>5.2616</v>
       </c>
       <c r="E4">
-        <v>0.9374</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="F4">
-        <v>0.1003</v>
+        <v>0.0891</v>
       </c>
       <c r="G4">
-        <v>0.0771</v>
+        <v>0.0741</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1907,22 +1907,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.868</v>
+        <v>5.7356</v>
       </c>
       <c r="C5">
-        <v>23.516</v>
+        <v>60.7155</v>
       </c>
       <c r="D5">
-        <v>4.8493</v>
+        <v>7.792</v>
       </c>
       <c r="E5">
-        <v>0.9715</v>
+        <v>0.9334</v>
       </c>
       <c r="F5">
-        <v>0.0907</v>
+        <v>0.1975</v>
       </c>
       <c r="G5">
-        <v>0.0735</v>
+        <v>0.1446</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1930,22 +1930,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.1452</v>
+        <v>4.0213</v>
       </c>
       <c r="C6">
-        <v>79.563</v>
+        <v>32.0038</v>
       </c>
       <c r="D6">
-        <v>8.9198</v>
+        <v>5.6572</v>
       </c>
       <c r="E6">
-        <v>0.8901</v>
+        <v>0.9513</v>
       </c>
       <c r="F6">
-        <v>0.1997</v>
+        <v>0.1077</v>
       </c>
       <c r="G6">
-        <v>0.1426</v>
+        <v>0.07630000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1953,22 +1953,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.6309</v>
+        <v>4.7252</v>
       </c>
       <c r="C7">
-        <v>43.2712</v>
+        <v>42.8909</v>
       </c>
       <c r="D7">
-        <v>6.4383</v>
+        <v>6.4799</v>
       </c>
       <c r="E7">
-        <v>0.9407</v>
+        <v>0.9436</v>
       </c>
       <c r="F7">
-        <v>0.1144</v>
+        <v>0.118</v>
       </c>
       <c r="G7">
-        <v>0.0868</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1976,22 +1976,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.7988</v>
+        <v>0.5956</v>
       </c>
       <c r="C8">
-        <v>19.0802</v>
+        <v>12.4008</v>
       </c>
       <c r="D8">
-        <v>1.3488</v>
+        <v>0.9494</v>
       </c>
       <c r="E8">
-        <v>0.0275</v>
+        <v>0.0122</v>
       </c>
       <c r="F8">
-        <v>0.0429</v>
+        <v>0.0406</v>
       </c>
       <c r="G8">
-        <v>0.0281</v>
+        <v>0.0278</v>
       </c>
     </row>
   </sheetData>
@@ -2035,22 +2035,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.2691</v>
+        <v>6.7322</v>
       </c>
       <c r="C2">
-        <v>50.2971</v>
+        <v>67.2937</v>
       </c>
       <c r="D2">
-        <v>7.092</v>
+        <v>8.2033</v>
       </c>
       <c r="E2">
-        <v>0.9308</v>
+        <v>0.9181</v>
       </c>
       <c r="F2">
-        <v>0.1152</v>
+        <v>0.1426</v>
       </c>
       <c r="G2">
-        <v>0.09089999999999999</v>
+        <v>0.1131</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2058,22 +2058,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.9616</v>
+        <v>5.1848</v>
       </c>
       <c r="C3">
-        <v>43.6126</v>
+        <v>49.8998</v>
       </c>
       <c r="D3">
-        <v>6.604</v>
+        <v>7.064</v>
       </c>
       <c r="E3">
-        <v>0.9467</v>
+        <v>0.9295</v>
       </c>
       <c r="F3">
-        <v>0.1034</v>
+        <v>0.1604</v>
       </c>
       <c r="G3">
-        <v>0.0857</v>
+        <v>0.1058</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2081,22 +2081,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.7887</v>
+        <v>6.0945</v>
       </c>
       <c r="C4">
-        <v>54.1168</v>
+        <v>53.8813</v>
       </c>
       <c r="D4">
-        <v>7.3564</v>
+        <v>7.3404</v>
       </c>
       <c r="E4">
-        <v>0.914</v>
+        <v>0.9186</v>
       </c>
       <c r="F4">
-        <v>0.1164</v>
+        <v>0.1291</v>
       </c>
       <c r="G4">
-        <v>0.0969</v>
+        <v>0.1077</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2104,22 +2104,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.2472</v>
+        <v>6.5391</v>
       </c>
       <c r="C5">
-        <v>37.3582</v>
+        <v>72.1733</v>
       </c>
       <c r="D5">
-        <v>6.1121</v>
+        <v>8.4955</v>
       </c>
       <c r="E5">
-        <v>0.9547</v>
+        <v>0.9208</v>
       </c>
       <c r="F5">
-        <v>0.1176</v>
+        <v>0.2117</v>
       </c>
       <c r="G5">
-        <v>0.101</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2127,22 +2127,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.5108</v>
+        <v>4.9277</v>
       </c>
       <c r="C6">
-        <v>80.4537</v>
+        <v>40.1634</v>
       </c>
       <c r="D6">
-        <v>8.9696</v>
+        <v>6.3375</v>
       </c>
       <c r="E6">
-        <v>0.8888</v>
+        <v>0.9389</v>
       </c>
       <c r="F6">
-        <v>0.2017</v>
+        <v>0.132</v>
       </c>
       <c r="G6">
-        <v>0.1522</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2150,22 +2150,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>5.5555</v>
+        <v>5.8957</v>
       </c>
       <c r="C7">
-        <v>53.1677</v>
+        <v>56.6823</v>
       </c>
       <c r="D7">
-        <v>7.2268</v>
+        <v>7.4881</v>
       </c>
       <c r="E7">
-        <v>0.927</v>
+        <v>0.9252</v>
       </c>
       <c r="F7">
-        <v>0.1308</v>
+        <v>0.1551</v>
       </c>
       <c r="G7">
-        <v>0.1053</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2173,22 +2173,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.5471</v>
+        <v>0.7205</v>
       </c>
       <c r="C8">
-        <v>14.798</v>
+        <v>11.6559</v>
       </c>
       <c r="D8">
-        <v>0.9698</v>
+        <v>0.7813</v>
       </c>
       <c r="E8">
-        <v>0.0236</v>
+        <v>0.008</v>
       </c>
       <c r="F8">
-        <v>0.0358</v>
+        <v>0.0303</v>
       </c>
       <c r="G8">
-        <v>0.024</v>
+        <v>0.0218</v>
       </c>
     </row>
   </sheetData>
@@ -2232,22 +2232,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.127</v>
+        <v>4.7849</v>
       </c>
       <c r="C2">
-        <v>31.3801</v>
+        <v>36.0137</v>
       </c>
       <c r="D2">
-        <v>5.6018</v>
+        <v>6.0011</v>
       </c>
       <c r="E2">
-        <v>0.9569</v>
+        <v>0.9562</v>
       </c>
       <c r="F2">
-        <v>0.0858</v>
+        <v>0.0872</v>
       </c>
       <c r="G2">
-        <v>0.0663</v>
+        <v>0.0736</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2255,22 +2255,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.0218</v>
+        <v>4.4661</v>
       </c>
       <c r="C3">
-        <v>29.6332</v>
+        <v>47.8932</v>
       </c>
       <c r="D3">
-        <v>5.4436</v>
+        <v>6.9205</v>
       </c>
       <c r="E3">
-        <v>0.9638</v>
+        <v>0.9324</v>
       </c>
       <c r="F3">
-        <v>0.08169999999999999</v>
+        <v>0.1016</v>
       </c>
       <c r="G3">
-        <v>0.06759999999999999</v>
+        <v>0.0757</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2278,22 +2278,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2125</v>
+        <v>4.3926</v>
       </c>
       <c r="C4">
-        <v>33.6663</v>
+        <v>28.0386</v>
       </c>
       <c r="D4">
-        <v>5.8023</v>
+        <v>5.2951</v>
       </c>
       <c r="E4">
-        <v>0.9465</v>
+        <v>0.9577</v>
       </c>
       <c r="F4">
-        <v>0.0924</v>
+        <v>0.09080000000000001</v>
       </c>
       <c r="G4">
-        <v>0.0707</v>
+        <v>0.0752</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2301,22 +2301,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.7362</v>
+        <v>5.4943</v>
       </c>
       <c r="C5">
-        <v>19.663</v>
+        <v>53.3835</v>
       </c>
       <c r="D5">
-        <v>4.4343</v>
+        <v>7.3064</v>
       </c>
       <c r="E5">
-        <v>0.9762</v>
+        <v>0.9415</v>
       </c>
       <c r="F5">
-        <v>0.08359999999999999</v>
+        <v>0.1802</v>
       </c>
       <c r="G5">
-        <v>0.0703</v>
+        <v>0.1332</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2324,22 +2324,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5.9907</v>
+        <v>3.8538</v>
       </c>
       <c r="C6">
-        <v>74.3045</v>
+        <v>29.3091</v>
       </c>
       <c r="D6">
-        <v>8.619999999999999</v>
+        <v>5.4138</v>
       </c>
       <c r="E6">
-        <v>0.8973</v>
+        <v>0.9554</v>
       </c>
       <c r="F6">
-        <v>0.1923</v>
+        <v>0.1047</v>
       </c>
       <c r="G6">
-        <v>0.138</v>
+        <v>0.07480000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2347,22 +2347,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.4177</v>
+        <v>4.5984</v>
       </c>
       <c r="C7">
-        <v>37.7294</v>
+        <v>38.9276</v>
       </c>
       <c r="D7">
-        <v>5.9804</v>
+        <v>6.1874</v>
       </c>
       <c r="E7">
-        <v>0.9481000000000001</v>
+        <v>0.9486</v>
       </c>
       <c r="F7">
-        <v>0.1072</v>
+        <v>0.1129</v>
       </c>
       <c r="G7">
-        <v>0.08260000000000001</v>
+        <v>0.08649999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2370,22 +2370,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.8028</v>
+        <v>0.5387999999999999</v>
       </c>
       <c r="C8">
-        <v>18.9024</v>
+        <v>10.0889</v>
       </c>
       <c r="D8">
-        <v>1.4015</v>
+        <v>0.8024</v>
       </c>
       <c r="E8">
-        <v>0.0272</v>
+        <v>0.01</v>
       </c>
       <c r="F8">
-        <v>0.0427</v>
+        <v>0.0343</v>
       </c>
       <c r="G8">
-        <v>0.0278</v>
+        <v>0.0234</v>
       </c>
     </row>
   </sheetData>
@@ -2429,22 +2429,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.1226</v>
+        <v>3.9086</v>
       </c>
       <c r="C2">
-        <v>30.4044</v>
+        <v>23.294</v>
       </c>
       <c r="D2">
-        <v>5.514</v>
+        <v>4.8264</v>
       </c>
       <c r="E2">
-        <v>0.9582000000000001</v>
+        <v>0.9717</v>
       </c>
       <c r="F2">
-        <v>0.09379999999999999</v>
+        <v>0.0643</v>
       </c>
       <c r="G2">
-        <v>0.06950000000000001</v>
+        <v>0.0563</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2452,22 +2452,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.0592</v>
+        <v>5.3399</v>
       </c>
       <c r="C3">
-        <v>27.9588</v>
+        <v>61.0785</v>
       </c>
       <c r="D3">
-        <v>5.2876</v>
+        <v>7.8153</v>
       </c>
       <c r="E3">
-        <v>0.9658</v>
+        <v>0.9137999999999999</v>
       </c>
       <c r="F3">
-        <v>0.0885</v>
+        <v>0.1114</v>
       </c>
       <c r="G3">
-        <v>0.0702</v>
+        <v>0.0851</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2475,22 +2475,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2494</v>
+        <v>4.1576</v>
       </c>
       <c r="C4">
-        <v>32.5908</v>
+        <v>26.6576</v>
       </c>
       <c r="D4">
-        <v>5.7088</v>
+        <v>5.1631</v>
       </c>
       <c r="E4">
-        <v>0.9482</v>
+        <v>0.9597</v>
       </c>
       <c r="F4">
-        <v>0.09</v>
+        <v>0.09030000000000001</v>
       </c>
       <c r="G4">
-        <v>0.0708</v>
+        <v>0.07290000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2498,22 +2498,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.1466</v>
+        <v>5.7948</v>
       </c>
       <c r="C5">
-        <v>16.0764</v>
+        <v>61.4996</v>
       </c>
       <c r="D5">
-        <v>4.0095</v>
+        <v>7.8422</v>
       </c>
       <c r="E5">
-        <v>0.9805</v>
+        <v>0.9326</v>
       </c>
       <c r="F5">
-        <v>0.07580000000000001</v>
+        <v>0.1865</v>
       </c>
       <c r="G5">
-        <v>0.0582</v>
+        <v>0.138</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2521,22 +2521,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.0815</v>
+        <v>3.7863</v>
       </c>
       <c r="C6">
-        <v>79.57170000000001</v>
+        <v>26.4179</v>
       </c>
       <c r="D6">
-        <v>8.920299999999999</v>
+        <v>5.1398</v>
       </c>
       <c r="E6">
-        <v>0.8901</v>
+        <v>0.9598</v>
       </c>
       <c r="F6">
-        <v>0.1887</v>
+        <v>0.1006</v>
       </c>
       <c r="G6">
-        <v>0.1348</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2544,22 +2544,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.3319</v>
+        <v>4.5974</v>
       </c>
       <c r="C7">
-        <v>37.3204</v>
+        <v>39.7895</v>
       </c>
       <c r="D7">
-        <v>5.8881</v>
+        <v>6.1574</v>
       </c>
       <c r="E7">
-        <v>0.9486</v>
+        <v>0.9475</v>
       </c>
       <c r="F7">
-        <v>0.1074</v>
+        <v>0.1106</v>
       </c>
       <c r="G7">
-        <v>0.08069999999999999</v>
+        <v>0.0848</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2567,22 +2567,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.9582000000000001</v>
+        <v>0.8137</v>
       </c>
       <c r="C8">
-        <v>21.883</v>
+        <v>17.5949</v>
       </c>
       <c r="D8">
-        <v>1.6282</v>
+        <v>1.3699</v>
       </c>
       <c r="E8">
-        <v>0.0311</v>
+        <v>0.0212</v>
       </c>
       <c r="F8">
-        <v>0.0411</v>
+        <v>0.041</v>
       </c>
       <c r="G8">
-        <v>0.0274</v>
+        <v>0.0281</v>
       </c>
     </row>
   </sheetData>
@@ -2629,22 +2629,22 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>4.4767</v>
+        <v>4.5871</v>
       </c>
       <c r="D2">
-        <v>29.2559</v>
+        <v>34.2862</v>
       </c>
       <c r="E2">
-        <v>5.4089</v>
+        <v>5.8554</v>
       </c>
       <c r="F2">
-        <v>0.9404</v>
+        <v>0.9308</v>
       </c>
       <c r="G2">
-        <v>0.08890000000000001</v>
+        <v>0.093</v>
       </c>
       <c r="H2">
-        <v>0.0751</v>
+        <v>0.07729999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the PPS & Corr Coeff figure size
</commit_message>
<xml_diff>
--- a/models/regression_model_1m/pycaret_tables.xlsx
+++ b/models/regression_model_1m/pycaret_tables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitProjects\springboard_capstone_1\Springboard_Capstone_01\models\regression_model_1m\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9836613C-B821-41C4-8B4F-D04084910F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="600" windowWidth="33540" windowHeight="19065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="compare_models" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
     <sheet name="pred_stack" sheetId="10" r:id="rId10"/>
     <sheet name="pred_final" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -182,8 +176,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,14 +240,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -300,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,27 +318,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,24 +352,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -577,27 +527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -631,28 +568,28 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>4.5075000000000003</v>
+        <v>4.5075</v>
       </c>
       <c r="D2">
-        <v>40.470999999999997</v>
+        <v>40.471</v>
       </c>
       <c r="E2">
-        <v>6.3150000000000004</v>
+        <v>6.315</v>
       </c>
       <c r="F2">
-        <v>0.94599999999999995</v>
+        <v>0.946</v>
       </c>
       <c r="G2">
         <v>0.115</v>
       </c>
       <c r="H2">
-        <v>8.4500000000000006E-2</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="I2">
-        <v>8.7999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -663,25 +600,25 @@
         <v>5.1025</v>
       </c>
       <c r="D3">
-        <v>48.241799999999998</v>
+        <v>48.2418</v>
       </c>
       <c r="E3">
-        <v>6.8486000000000002</v>
+        <v>6.8486</v>
       </c>
       <c r="F3">
-        <v>0.93540000000000001</v>
+        <v>0.9354</v>
       </c>
       <c r="G3">
         <v>0.1201</v>
       </c>
       <c r="H3">
-        <v>9.2399999999999996E-2</v>
+        <v>0.0924</v>
       </c>
       <c r="I3">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.054</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -689,28 +626,28 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <v>5.2172999999999998</v>
+        <v>5.2173</v>
       </c>
       <c r="D4">
-        <v>53.365299999999998</v>
+        <v>53.3653</v>
       </c>
       <c r="E4">
-        <v>7.2457000000000003</v>
+        <v>7.2457</v>
       </c>
       <c r="F4">
-        <v>0.92889999999999995</v>
+        <v>0.9288999999999999</v>
       </c>
       <c r="G4">
-        <v>0.12230000000000001</v>
+        <v>0.1223</v>
       </c>
       <c r="H4">
-        <v>9.3299999999999994E-2</v>
+        <v>0.09329999999999999</v>
       </c>
       <c r="I4">
-        <v>3.5999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -718,28 +655,28 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>5.2953999999999999</v>
+        <v>5.2954</v>
       </c>
       <c r="D5">
-        <v>55.055599999999998</v>
+        <v>55.0556</v>
       </c>
       <c r="E5">
-        <v>7.3762999999999996</v>
+        <v>7.3763</v>
       </c>
       <c r="F5">
-        <v>0.92610000000000003</v>
+        <v>0.9261</v>
       </c>
       <c r="G5">
-        <v>0.12989999999999999</v>
+        <v>0.1299</v>
       </c>
       <c r="H5">
-        <v>9.6199999999999994E-2</v>
+        <v>0.09619999999999999</v>
       </c>
       <c r="I5">
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -747,28 +684,28 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>5.8956999999999997</v>
+        <v>5.8957</v>
       </c>
       <c r="D6">
-        <v>56.682299999999998</v>
+        <v>56.6823</v>
       </c>
       <c r="E6">
-        <v>7.4881000000000002</v>
+        <v>7.4881</v>
       </c>
       <c r="F6">
-        <v>0.92520000000000002</v>
+        <v>0.9252</v>
       </c>
       <c r="G6">
-        <v>0.15509999999999999</v>
+        <v>0.1551</v>
       </c>
       <c r="H6">
-        <v>0.11799999999999999</v>
+        <v>0.118</v>
       </c>
       <c r="I6">
-        <v>1.4039999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -776,16 +713,16 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>5.7991000000000001</v>
+        <v>5.7991</v>
       </c>
       <c r="D7">
         <v>59.5745</v>
       </c>
       <c r="E7">
-        <v>7.6262999999999996</v>
+        <v>7.6263</v>
       </c>
       <c r="F7">
-        <v>0.92049999999999998</v>
+        <v>0.9205</v>
       </c>
       <c r="G7">
         <v>0.1333</v>
@@ -794,10 +731,10 @@
         <v>0.1076</v>
       </c>
       <c r="I7">
-        <v>5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.052</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -805,28 +742,28 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>5.8053999999999997</v>
+        <v>5.8054</v>
       </c>
       <c r="D8">
-        <v>58.890300000000003</v>
+        <v>58.8903</v>
       </c>
       <c r="E8">
-        <v>7.6360999999999999</v>
+        <v>7.6361</v>
       </c>
       <c r="F8">
-        <v>0.92220000000000002</v>
+        <v>0.9222</v>
       </c>
       <c r="G8">
-        <v>0.15690000000000001</v>
+        <v>0.1569</v>
       </c>
       <c r="H8">
         <v>0.1162</v>
       </c>
       <c r="I8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -834,16 +771,16 @@
         <v>33</v>
       </c>
       <c r="C9">
-        <v>5.9442000000000004</v>
+        <v>5.9442</v>
       </c>
       <c r="D9">
-        <v>59.675800000000002</v>
+        <v>59.6758</v>
       </c>
       <c r="E9">
-        <v>7.6896000000000004</v>
+        <v>7.6896</v>
       </c>
       <c r="F9">
-        <v>0.92069999999999996</v>
+        <v>0.9207</v>
       </c>
       <c r="G9">
         <v>0.155</v>
@@ -852,10 +789,10 @@
         <v>0.1166</v>
       </c>
       <c r="I9">
-        <v>2.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -863,28 +800,28 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>6.0204000000000004</v>
+        <v>6.0204</v>
       </c>
       <c r="D10">
         <v>62.5989</v>
       </c>
       <c r="E10">
-        <v>7.8761000000000001</v>
+        <v>7.8761</v>
       </c>
       <c r="F10">
-        <v>0.91649999999999998</v>
+        <v>0.9165</v>
       </c>
       <c r="G10">
-        <v>0.15840000000000001</v>
+        <v>0.1584</v>
       </c>
       <c r="H10">
         <v>0.1173</v>
       </c>
       <c r="I10">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -892,16 +829,16 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>6.2584999999999997</v>
+        <v>6.2585</v>
       </c>
       <c r="D11">
-        <v>68.050799999999995</v>
+        <v>68.0508</v>
       </c>
       <c r="E11">
-        <v>8.2174999999999994</v>
+        <v>8.217499999999999</v>
       </c>
       <c r="F11">
-        <v>0.90939999999999999</v>
+        <v>0.9094</v>
       </c>
       <c r="G11">
         <v>0.1603</v>
@@ -910,10 +847,10 @@
         <v>0.1227</v>
       </c>
       <c r="I11">
-        <v>0.82199999999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -924,25 +861,25 @@
         <v>5.8895</v>
       </c>
       <c r="D12">
-        <v>73.736500000000007</v>
+        <v>73.73650000000001</v>
       </c>
       <c r="E12">
-        <v>8.4239999999999995</v>
+        <v>8.423999999999999</v>
       </c>
       <c r="F12">
-        <v>0.90469999999999995</v>
+        <v>0.9046999999999999</v>
       </c>
       <c r="G12">
-        <v>0.14149999999999999</v>
+        <v>0.1415</v>
       </c>
       <c r="H12">
-        <v>0.10920000000000001</v>
+        <v>0.1092</v>
       </c>
       <c r="I12">
-        <v>2.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -950,28 +887,28 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>6.3057999999999996</v>
+        <v>6.3058</v>
       </c>
       <c r="D13">
-        <v>75.900700000000001</v>
+        <v>75.9007</v>
       </c>
       <c r="E13">
-        <v>8.6956000000000007</v>
+        <v>8.695600000000001</v>
       </c>
       <c r="F13">
         <v>0.8972</v>
       </c>
       <c r="G13">
-        <v>0.16969999999999999</v>
+        <v>0.1697</v>
       </c>
       <c r="H13">
         <v>0.1241</v>
       </c>
       <c r="I13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -979,28 +916,28 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>6.8563000000000001</v>
+        <v>6.8563</v>
       </c>
       <c r="D14">
-        <v>79.070999999999998</v>
+        <v>79.071</v>
       </c>
       <c r="E14">
-        <v>8.8598999999999997</v>
+        <v>8.8599</v>
       </c>
       <c r="F14">
-        <v>0.89490000000000003</v>
+        <v>0.8949</v>
       </c>
       <c r="G14">
-        <v>0.16569999999999999</v>
+        <v>0.1657</v>
       </c>
       <c r="H14">
-        <v>0.13250000000000001</v>
+        <v>0.1325</v>
       </c>
       <c r="I14">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1008,28 +945,28 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>6.6426999999999996</v>
+        <v>6.6427</v>
       </c>
       <c r="D15">
-        <v>84.368399999999994</v>
+        <v>84.36839999999999</v>
       </c>
       <c r="E15">
-        <v>9.0701999999999998</v>
+        <v>9.0702</v>
       </c>
       <c r="F15">
-        <v>0.88419999999999999</v>
+        <v>0.8842</v>
       </c>
       <c r="G15">
-        <v>0.15359999999999999</v>
+        <v>0.1536</v>
       </c>
       <c r="H15">
         <v>0.1183</v>
       </c>
       <c r="I15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1037,28 +974,28 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>8.6614000000000004</v>
+        <v>8.6614</v>
       </c>
       <c r="D16">
         <v>132.6311</v>
       </c>
       <c r="E16">
-        <v>10.896599999999999</v>
+        <v>10.8966</v>
       </c>
       <c r="F16">
-        <v>0.81769999999999998</v>
+        <v>0.8177</v>
       </c>
       <c r="G16">
-        <v>0.31490000000000001</v>
+        <v>0.3149</v>
       </c>
       <c r="H16">
-        <v>0.18840000000000001</v>
+        <v>0.1884</v>
       </c>
       <c r="I16">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1075,19 +1012,19 @@
         <v>15.7637</v>
       </c>
       <c r="F17">
-        <v>0.66769999999999996</v>
+        <v>0.6677</v>
       </c>
       <c r="G17">
-        <v>0.27950000000000003</v>
+        <v>0.2795</v>
       </c>
       <c r="H17">
-        <v>0.26429999999999998</v>
+        <v>0.2643</v>
       </c>
       <c r="I17">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1095,28 +1032,28 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>23.206800000000001</v>
+        <v>23.2068</v>
       </c>
       <c r="D18">
-        <v>756.93460000000005</v>
+        <v>756.9346</v>
       </c>
       <c r="E18">
-        <v>27.450800000000001</v>
+        <v>27.4508</v>
       </c>
       <c r="F18">
-        <v>-5.5999999999999999E-3</v>
+        <v>-0.0056</v>
       </c>
       <c r="G18">
-        <v>0.47820000000000001</v>
+        <v>0.4782</v>
       </c>
       <c r="H18">
-        <v>0.49559999999999998</v>
+        <v>0.4956</v>
       </c>
       <c r="I18">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1124,25 +1061,25 @@
         <v>43</v>
       </c>
       <c r="C19">
-        <v>4382.0176000000001</v>
+        <v>4382.0176</v>
       </c>
       <c r="D19">
-        <v>192874824.18599999</v>
+        <v>192874824.186</v>
       </c>
       <c r="E19">
-        <v>6358.1619000000001</v>
+        <v>6358.1619</v>
       </c>
       <c r="F19">
-        <v>-272295.77159999998</v>
+        <v>-272295.7716</v>
       </c>
       <c r="G19">
-        <v>1.8958999999999999</v>
+        <v>1.8959</v>
       </c>
       <c r="H19">
-        <v>75.491500000000002</v>
+        <v>75.4915</v>
       </c>
       <c r="I19">
-        <v>2.4E-2</v>
+        <v>0.022</v>
       </c>
     </row>
   </sheetData>
@@ -1151,14 +1088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1189,22 +1126,22 @@
         <v>48</v>
       </c>
       <c r="C2">
-        <v>5.2774999999999999</v>
+        <v>5.2775</v>
       </c>
       <c r="D2">
-        <v>44.208100000000002</v>
+        <v>44.2081</v>
       </c>
       <c r="E2">
-        <v>6.6489000000000003</v>
+        <v>6.6489</v>
       </c>
       <c r="F2">
-        <v>0.91069999999999995</v>
+        <v>0.9107</v>
       </c>
       <c r="G2">
         <v>0.1042</v>
       </c>
       <c r="H2">
-        <v>8.8099999999999998E-2</v>
+        <v>0.0881</v>
       </c>
     </row>
   </sheetData>
@@ -1213,14 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1251,7 +1188,7 @@
         <v>48</v>
       </c>
       <c r="C2">
-        <v>0.98280000000000001</v>
+        <v>0.9828</v>
       </c>
       <c r="D2">
         <v>1.9863</v>
@@ -1260,13 +1197,13 @@
         <v>1.4094</v>
       </c>
       <c r="F2">
-        <v>0.99709999999999999</v>
+        <v>0.9971</v>
       </c>
       <c r="G2">
-        <v>2.46E-2</v>
+        <v>0.0246</v>
       </c>
       <c r="H2">
-        <v>1.6400000000000001E-2</v>
+        <v>0.0164</v>
       </c>
     </row>
   </sheetData>
@@ -1275,14 +1212,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1305,122 +1242,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.4767000000000001</v>
+        <v>4.4767</v>
       </c>
       <c r="C2">
-        <v>35.624400000000001</v>
+        <v>35.6244</v>
       </c>
       <c r="D2">
-        <v>5.9686000000000003</v>
+        <v>5.9686</v>
       </c>
       <c r="E2">
-        <v>0.95669999999999999</v>
+        <v>0.9567</v>
       </c>
       <c r="F2">
-        <v>8.0399999999999999E-2</v>
+        <v>0.0804</v>
       </c>
       <c r="G2">
-        <v>6.7599999999999993E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.06759999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.6015999999999999</v>
+        <v>3.6016</v>
       </c>
       <c r="C3">
-        <v>36.618200000000002</v>
+        <v>36.6182</v>
       </c>
       <c r="D3">
-        <v>6.0513000000000003</v>
+        <v>6.0513</v>
       </c>
       <c r="E3">
-        <v>0.94830000000000003</v>
+        <v>0.9483</v>
       </c>
       <c r="F3">
-        <v>8.8900000000000007E-2</v>
+        <v>0.08890000000000001</v>
       </c>
       <c r="G3">
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.3482000000000003</v>
+        <v>4.3482</v>
       </c>
       <c r="C4">
         <v>31.7973</v>
       </c>
       <c r="D4">
-        <v>5.6388999999999996</v>
+        <v>5.6389</v>
       </c>
       <c r="E4">
-        <v>0.95199999999999996</v>
+        <v>0.952</v>
       </c>
       <c r="F4">
-        <v>8.4400000000000003E-2</v>
+        <v>0.0844</v>
       </c>
       <c r="G4">
-        <v>7.22E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.4470000000000001</v>
+        <v>6.447</v>
       </c>
       <c r="C5">
-        <v>80.987899999999996</v>
+        <v>80.9879</v>
       </c>
       <c r="D5">
-        <v>8.9992999999999999</v>
+        <v>8.9993</v>
       </c>
       <c r="E5">
-        <v>0.91120000000000001</v>
+        <v>0.9112</v>
       </c>
       <c r="F5">
-        <v>0.21679999999999999</v>
+        <v>0.2168</v>
       </c>
       <c r="G5">
         <v>0.1636</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.2916999999999996</v>
+        <v>4.2917</v>
       </c>
       <c r="C6">
         <v>38.2074</v>
       </c>
       <c r="D6">
-        <v>6.1811999999999996</v>
+        <v>6.1812</v>
       </c>
       <c r="E6">
-        <v>0.94189999999999996</v>
+        <v>0.9419</v>
       </c>
       <c r="F6">
         <v>0.115</v>
       </c>
       <c r="G6">
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.081</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1428,42 +1365,42 @@
         <v>4.633</v>
       </c>
       <c r="C7">
-        <v>44.646999999999998</v>
+        <v>44.647</v>
       </c>
       <c r="D7">
-        <v>6.5678999999999998</v>
+        <v>6.5679</v>
       </c>
       <c r="E7">
-        <v>0.94199999999999995</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F7">
         <v>0.1171</v>
       </c>
       <c r="G7">
-        <v>8.8900000000000007E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.08890000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.95669999999999999</v>
+        <v>0.9567</v>
       </c>
       <c r="C8">
         <v>18.2927</v>
       </c>
       <c r="D8">
-        <v>1.2289000000000001</v>
+        <v>1.2289</v>
       </c>
       <c r="E8">
-        <v>1.6199999999999999E-2</v>
+        <v>0.0162</v>
       </c>
       <c r="F8">
-        <v>5.1299999999999998E-2</v>
+        <v>0.0513</v>
       </c>
       <c r="G8">
-        <v>3.7999999999999999E-2</v>
+        <v>0.038</v>
       </c>
     </row>
   </sheetData>
@@ -1472,14 +1409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1502,53 +1439,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.6779000000000002</v>
+        <v>4.6779</v>
       </c>
       <c r="C2">
-        <v>34.332799999999999</v>
+        <v>34.3328</v>
       </c>
       <c r="D2">
-        <v>5.8593999999999999</v>
+        <v>5.8594</v>
       </c>
       <c r="E2">
-        <v>0.95820000000000005</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="F2">
-        <v>8.8700000000000001E-2</v>
+        <v>0.0887</v>
       </c>
       <c r="G2">
-        <v>7.3300000000000004E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0733</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.3189000000000002</v>
+        <v>5.3189</v>
       </c>
       <c r="C3">
-        <v>59.473599999999998</v>
+        <v>59.4736</v>
       </c>
       <c r="D3">
         <v>7.7119</v>
       </c>
       <c r="E3">
-        <v>0.91600000000000004</v>
+        <v>0.916</v>
       </c>
       <c r="F3">
-        <v>0.11459999999999999</v>
+        <v>0.1146</v>
       </c>
       <c r="G3">
-        <v>8.9099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1556,27 +1493,27 @@
         <v>3.875</v>
       </c>
       <c r="C4">
-        <v>23.571000000000002</v>
+        <v>23.571</v>
       </c>
       <c r="D4">
-        <v>4.8550000000000004</v>
+        <v>4.855</v>
       </c>
       <c r="E4">
-        <v>0.96440000000000003</v>
+        <v>0.9644</v>
       </c>
       <c r="F4">
-        <v>9.1899999999999996E-2</v>
+        <v>0.0919</v>
       </c>
       <c r="G4">
-        <v>6.9900000000000004E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.5547000000000004</v>
+        <v>5.5547</v>
       </c>
       <c r="C5">
         <v>57.3705</v>
@@ -1585,7 +1522,7 @@
         <v>7.5743</v>
       </c>
       <c r="E5">
-        <v>0.93710000000000004</v>
+        <v>0.9371</v>
       </c>
       <c r="F5">
         <v>0.188</v>
@@ -1594,73 +1531,73 @@
         <v>0.1366</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.3128000000000002</v>
+        <v>3.3128</v>
       </c>
       <c r="C6">
         <v>20.7651</v>
       </c>
       <c r="D6">
-        <v>4.5568999999999997</v>
+        <v>4.5569</v>
       </c>
       <c r="E6">
-        <v>0.96840000000000004</v>
+        <v>0.9684</v>
       </c>
       <c r="F6">
-        <v>8.8400000000000006E-2</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="G6">
-        <v>6.2600000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0626</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5479000000000003</v>
+        <v>4.5479</v>
       </c>
       <c r="C7">
-        <v>39.102600000000002</v>
+        <v>39.1026</v>
       </c>
       <c r="D7">
-        <v>6.1115000000000004</v>
+        <v>6.1115</v>
       </c>
       <c r="E7">
-        <v>0.94879999999999998</v>
+        <v>0.9488</v>
       </c>
       <c r="F7">
         <v>0.1143</v>
       </c>
       <c r="G7">
-        <v>8.6300000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.84889999999999999</v>
+        <v>0.8489</v>
       </c>
       <c r="C8">
         <v>16.4252</v>
       </c>
       <c r="D8">
-        <v>1.3237000000000001</v>
+        <v>1.3237</v>
       </c>
       <c r="E8">
-        <v>1.9599999999999999E-2</v>
+        <v>0.0196</v>
       </c>
       <c r="F8">
-        <v>3.8100000000000002E-2</v>
+        <v>0.0381</v>
       </c>
       <c r="G8">
-        <v>2.6599999999999999E-2</v>
+        <v>0.0266</v>
       </c>
     </row>
   </sheetData>
@@ -1669,14 +1606,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1699,122 +1636,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.0395000000000003</v>
+        <v>5.0395</v>
       </c>
       <c r="C2">
-        <v>45.962400000000002</v>
+        <v>45.9624</v>
       </c>
       <c r="D2">
-        <v>6.7796000000000003</v>
+        <v>6.7796</v>
       </c>
       <c r="E2">
-        <v>0.94410000000000005</v>
+        <v>0.9441000000000001</v>
       </c>
       <c r="F2">
-        <v>9.6799999999999997E-2</v>
+        <v>0.0968</v>
       </c>
       <c r="G2">
-        <v>7.6499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0765</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.2367999999999997</v>
+        <v>5.2368</v>
       </c>
       <c r="C3">
-        <v>63.589300000000001</v>
+        <v>63.5893</v>
       </c>
       <c r="D3">
-        <v>7.9743000000000004</v>
+        <v>7.9743</v>
       </c>
       <c r="E3">
-        <v>0.91020000000000001</v>
+        <v>0.9102</v>
       </c>
       <c r="F3">
         <v>0.1152</v>
       </c>
       <c r="G3">
-        <v>8.6699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0867</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.6567999999999996</v>
+        <v>4.6568</v>
       </c>
       <c r="C4">
-        <v>32.516100000000002</v>
+        <v>32.5161</v>
       </c>
       <c r="D4">
-        <v>5.7023000000000001</v>
+        <v>5.7023</v>
       </c>
       <c r="E4">
-        <v>0.95089999999999997</v>
+        <v>0.9509</v>
       </c>
       <c r="F4">
-        <v>0.10290000000000001</v>
+        <v>0.1029</v>
       </c>
       <c r="G4">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.079</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.6616999999999997</v>
+        <v>5.6617</v>
       </c>
       <c r="C5">
-        <v>57.065899999999999</v>
+        <v>57.0659</v>
       </c>
       <c r="D5">
-        <v>7.5541999999999998</v>
+        <v>7.5542</v>
       </c>
       <c r="E5">
-        <v>0.93740000000000001</v>
+        <v>0.9374</v>
       </c>
       <c r="F5">
-        <v>0.17730000000000001</v>
+        <v>0.1773</v>
       </c>
       <c r="G5">
-        <v>0.13400000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5.0891000000000002</v>
+        <v>5.0891</v>
       </c>
       <c r="C6">
-        <v>46.352499999999999</v>
+        <v>46.3525</v>
       </c>
       <c r="D6">
         <v>6.8083</v>
       </c>
       <c r="E6">
-        <v>0.92949999999999999</v>
+        <v>0.9295</v>
       </c>
       <c r="F6">
         <v>0.1196</v>
       </c>
       <c r="G6">
-        <v>9.11E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0911</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1822,42 +1759,42 @@
         <v>5.1368</v>
       </c>
       <c r="C7">
-        <v>49.097200000000001</v>
+        <v>49.0972</v>
       </c>
       <c r="D7">
-        <v>6.9637000000000002</v>
+        <v>6.9637</v>
       </c>
       <c r="E7">
-        <v>0.93440000000000001</v>
+        <v>0.9344</v>
       </c>
       <c r="F7">
-        <v>0.12239999999999999</v>
+        <v>0.1224</v>
       </c>
       <c r="G7">
-        <v>9.35E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0935</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.32479999999999998</v>
+        <v>0.3248</v>
       </c>
       <c r="C8">
         <v>10.6378</v>
       </c>
       <c r="D8">
-        <v>0.77710000000000001</v>
+        <v>0.7771</v>
       </c>
       <c r="E8">
-        <v>1.4E-2</v>
+        <v>0.014</v>
       </c>
       <c r="F8">
-        <v>2.87E-2</v>
+        <v>0.0287</v>
       </c>
       <c r="G8">
-        <v>2.0899999999999998E-2</v>
+        <v>0.0209</v>
       </c>
     </row>
   </sheetData>
@@ -1866,16 +1803,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1898,41 +1833,41 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.8396999999999997</v>
+        <v>4.8397</v>
       </c>
       <c r="C2">
-        <v>41.226799999999997</v>
+        <v>41.2268</v>
       </c>
       <c r="D2">
-        <v>6.4207999999999998</v>
+        <v>6.4208</v>
       </c>
       <c r="E2">
-        <v>0.94979999999999998</v>
+        <v>0.9498</v>
       </c>
       <c r="F2">
-        <v>8.8400000000000006E-2</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="G2">
-        <v>7.2900000000000006E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.07290000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.7934999999999999</v>
+        <v>4.7935</v>
       </c>
       <c r="C3">
-        <v>52.823599999999999</v>
+        <v>52.8236</v>
       </c>
       <c r="D3">
-        <v>7.2679999999999998</v>
+        <v>7.268</v>
       </c>
       <c r="E3">
         <v>0.9254</v>
@@ -1941,122 +1876,122 @@
         <v>0.1071</v>
       </c>
       <c r="G3">
-        <v>7.7399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0774</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2358000000000002</v>
+        <v>4.2358</v>
       </c>
       <c r="C4">
-        <v>27.684899999999999</v>
+        <v>27.6849</v>
       </c>
       <c r="D4">
-        <v>5.2615999999999996</v>
+        <v>5.2616</v>
       </c>
       <c r="E4">
-        <v>0.95820000000000005</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="F4">
-        <v>8.9099999999999999E-2</v>
+        <v>0.0891</v>
       </c>
       <c r="G4">
-        <v>7.4099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0741</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.7355999999999998</v>
+        <v>5.7356</v>
       </c>
       <c r="C5">
-        <v>60.715499999999999</v>
+        <v>60.7155</v>
       </c>
       <c r="D5">
-        <v>7.7919999999999998</v>
+        <v>7.792</v>
       </c>
       <c r="E5">
-        <v>0.93340000000000001</v>
+        <v>0.9334</v>
       </c>
       <c r="F5">
-        <v>0.19750000000000001</v>
+        <v>0.1975</v>
       </c>
       <c r="G5">
-        <v>0.14460000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.0213000000000001</v>
+        <v>4.0213</v>
       </c>
       <c r="C6">
-        <v>32.003799999999998</v>
+        <v>32.0038</v>
       </c>
       <c r="D6">
-        <v>5.6571999999999996</v>
+        <v>5.6572</v>
       </c>
       <c r="E6">
-        <v>0.95130000000000003</v>
+        <v>0.9513</v>
       </c>
       <c r="F6">
         <v>0.1077</v>
       </c>
       <c r="G6">
-        <v>7.6300000000000007E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.07630000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.7252000000000001</v>
+        <v>4.7252</v>
       </c>
       <c r="C7">
-        <v>42.890900000000002</v>
+        <v>42.8909</v>
       </c>
       <c r="D7">
-        <v>6.4798999999999998</v>
+        <v>6.4799</v>
       </c>
       <c r="E7">
-        <v>0.94359999999999999</v>
+        <v>0.9436</v>
       </c>
       <c r="F7">
-        <v>0.11799999999999999</v>
+        <v>0.118</v>
       </c>
       <c r="G7">
-        <v>8.9099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.59560000000000002</v>
+        <v>0.5956</v>
       </c>
       <c r="C8">
         <v>12.4008</v>
       </c>
       <c r="D8">
-        <v>0.94940000000000002</v>
+        <v>0.9494</v>
       </c>
       <c r="E8">
-        <v>1.2200000000000001E-2</v>
+        <v>0.0122</v>
       </c>
       <c r="F8">
-        <v>4.0599999999999997E-2</v>
+        <v>0.0406</v>
       </c>
       <c r="G8">
-        <v>2.7799999999999998E-2</v>
+        <v>0.0278</v>
       </c>
     </row>
   </sheetData>
@@ -2065,14 +2000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2095,53 +2030,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6.7321999999999997</v>
+        <v>6.7322</v>
       </c>
       <c r="C2">
-        <v>67.293700000000001</v>
+        <v>67.2937</v>
       </c>
       <c r="D2">
-        <v>8.2033000000000005</v>
+        <v>8.2033</v>
       </c>
       <c r="E2">
-        <v>0.91810000000000003</v>
+        <v>0.9181</v>
       </c>
       <c r="F2">
         <v>0.1426</v>
       </c>
       <c r="G2">
-        <v>0.11310000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.1848000000000001</v>
+        <v>5.1848</v>
       </c>
       <c r="C3">
-        <v>49.899799999999999</v>
+        <v>49.8998</v>
       </c>
       <c r="D3">
-        <v>7.0640000000000001</v>
+        <v>7.064</v>
       </c>
       <c r="E3">
-        <v>0.92949999999999999</v>
+        <v>0.9295</v>
       </c>
       <c r="F3">
-        <v>0.16039999999999999</v>
+        <v>0.1604</v>
       </c>
       <c r="G3">
-        <v>0.10580000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1058</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2149,36 +2084,36 @@
         <v>6.0945</v>
       </c>
       <c r="C4">
-        <v>53.881300000000003</v>
+        <v>53.8813</v>
       </c>
       <c r="D4">
-        <v>7.3403999999999998</v>
+        <v>7.3404</v>
       </c>
       <c r="E4">
-        <v>0.91859999999999997</v>
+        <v>0.9186</v>
       </c>
       <c r="F4">
-        <v>0.12909999999999999</v>
+        <v>0.1291</v>
       </c>
       <c r="G4">
         <v>0.1077</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.5391000000000004</v>
+        <v>6.5391</v>
       </c>
       <c r="C5">
-        <v>72.173299999999998</v>
+        <v>72.1733</v>
       </c>
       <c r="D5">
-        <v>8.4954999999999998</v>
+        <v>8.4955</v>
       </c>
       <c r="E5">
-        <v>0.92079999999999995</v>
+        <v>0.9208</v>
       </c>
       <c r="F5">
         <v>0.2117</v>
@@ -2187,73 +2122,73 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.9276999999999997</v>
+        <v>4.9277</v>
       </c>
       <c r="C6">
-        <v>40.163400000000003</v>
+        <v>40.1634</v>
       </c>
       <c r="D6">
-        <v>6.3375000000000004</v>
+        <v>6.3375</v>
       </c>
       <c r="E6">
-        <v>0.93889999999999996</v>
+        <v>0.9389</v>
       </c>
       <c r="F6">
-        <v>0.13200000000000001</v>
+        <v>0.132</v>
       </c>
       <c r="G6">
         <v>0.1022</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7">
-        <v>5.8956999999999997</v>
+        <v>5.8957</v>
       </c>
       <c r="C7">
-        <v>56.682299999999998</v>
+        <v>56.6823</v>
       </c>
       <c r="D7">
-        <v>7.4881000000000002</v>
+        <v>7.4881</v>
       </c>
       <c r="E7">
-        <v>0.92520000000000002</v>
+        <v>0.9252</v>
       </c>
       <c r="F7">
-        <v>0.15509999999999999</v>
+        <v>0.1551</v>
       </c>
       <c r="G7">
-        <v>0.11799999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.72050000000000003</v>
+        <v>0.7205</v>
       </c>
       <c r="C8">
-        <v>11.655900000000001</v>
+        <v>11.6559</v>
       </c>
       <c r="D8">
-        <v>0.78129999999999999</v>
+        <v>0.7813</v>
       </c>
       <c r="E8">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="F8">
-        <v>3.0300000000000001E-2</v>
+        <v>0.0303</v>
       </c>
       <c r="G8">
-        <v>2.18E-2</v>
+        <v>0.0218</v>
       </c>
     </row>
   </sheetData>
@@ -2262,14 +2197,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2292,30 +2227,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.7849000000000004</v>
+        <v>4.7849</v>
       </c>
       <c r="C2">
         <v>36.0137</v>
       </c>
       <c r="D2">
-        <v>6.0011000000000001</v>
+        <v>6.0011</v>
       </c>
       <c r="E2">
-        <v>0.95620000000000005</v>
+        <v>0.9562</v>
       </c>
       <c r="F2">
-        <v>8.72E-2</v>
+        <v>0.0872</v>
       </c>
       <c r="G2">
-        <v>7.3599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2326,42 +2261,42 @@
         <v>47.8932</v>
       </c>
       <c r="D3">
-        <v>6.9204999999999997</v>
+        <v>6.9205</v>
       </c>
       <c r="E3">
-        <v>0.93240000000000001</v>
+        <v>0.9324</v>
       </c>
       <c r="F3">
         <v>0.1016</v>
       </c>
       <c r="G3">
-        <v>7.5700000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0757</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.3925999999999998</v>
+        <v>4.3926</v>
       </c>
       <c r="C4">
-        <v>28.038599999999999</v>
+        <v>28.0386</v>
       </c>
       <c r="D4">
-        <v>5.2950999999999997</v>
+        <v>5.2951</v>
       </c>
       <c r="E4">
         <v>0.9577</v>
       </c>
       <c r="F4">
-        <v>9.0800000000000006E-2</v>
+        <v>0.09080000000000001</v>
       </c>
       <c r="G4">
-        <v>7.5200000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2369,7 +2304,7 @@
         <v>5.4943</v>
       </c>
       <c r="C5">
-        <v>53.383499999999998</v>
+        <v>53.3835</v>
       </c>
       <c r="D5">
         <v>7.3064</v>
@@ -2381,44 +2316,44 @@
         <v>0.1802</v>
       </c>
       <c r="G5">
-        <v>0.13320000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.8538000000000001</v>
+        <v>3.8538</v>
       </c>
       <c r="C6">
-        <v>29.309100000000001</v>
+        <v>29.3091</v>
       </c>
       <c r="D6">
-        <v>5.4138000000000002</v>
+        <v>5.4138</v>
       </c>
       <c r="E6">
-        <v>0.95540000000000003</v>
+        <v>0.9554</v>
       </c>
       <c r="F6">
         <v>0.1047</v>
       </c>
       <c r="G6">
-        <v>7.4800000000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.07480000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5983999999999998</v>
+        <v>4.5984</v>
       </c>
       <c r="C7">
-        <v>38.927599999999998</v>
+        <v>38.9276</v>
       </c>
       <c r="D7">
-        <v>6.1874000000000002</v>
+        <v>6.1874</v>
       </c>
       <c r="E7">
         <v>0.9486</v>
@@ -2427,18 +2362,18 @@
         <v>0.1129</v>
       </c>
       <c r="G7">
-        <v>8.6499999999999994E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.08649999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.53879999999999995</v>
+        <v>0.5387999999999999</v>
       </c>
       <c r="C8">
-        <v>10.088900000000001</v>
+        <v>10.0889</v>
       </c>
       <c r="D8">
         <v>0.8024</v>
@@ -2447,10 +2382,10 @@
         <v>0.01</v>
       </c>
       <c r="F8">
-        <v>3.4299999999999997E-2</v>
+        <v>0.0343</v>
       </c>
       <c r="G8">
-        <v>2.3400000000000001E-2</v>
+        <v>0.0234</v>
       </c>
     </row>
   </sheetData>
@@ -2459,14 +2394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2489,61 +2424,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.9085999999999999</v>
+        <v>3.9086</v>
       </c>
       <c r="C2">
         <v>23.294</v>
       </c>
       <c r="D2">
-        <v>4.8263999999999996</v>
+        <v>4.8264</v>
       </c>
       <c r="E2">
-        <v>0.97170000000000001</v>
+        <v>0.9717</v>
       </c>
       <c r="F2">
-        <v>6.4299999999999996E-2</v>
+        <v>0.0643</v>
       </c>
       <c r="G2">
-        <v>5.6300000000000003E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.3399000000000001</v>
+        <v>5.3399</v>
       </c>
       <c r="C3">
-        <v>61.078499999999998</v>
+        <v>61.0785</v>
       </c>
       <c r="D3">
-        <v>7.8152999999999997</v>
+        <v>7.8153</v>
       </c>
       <c r="E3">
-        <v>0.91379999999999995</v>
+        <v>0.9137999999999999</v>
       </c>
       <c r="F3">
         <v>0.1114</v>
       </c>
       <c r="G3">
-        <v>8.5099999999999995E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.1576000000000004</v>
+        <v>4.1576</v>
       </c>
       <c r="C4">
-        <v>26.657599999999999</v>
+        <v>26.6576</v>
       </c>
       <c r="D4">
         <v>5.1631</v>
@@ -2552,102 +2487,102 @@
         <v>0.9597</v>
       </c>
       <c r="F4">
-        <v>9.0300000000000005E-2</v>
+        <v>0.09030000000000001</v>
       </c>
       <c r="G4">
-        <v>7.2900000000000006E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.07290000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.7948000000000004</v>
+        <v>5.7948</v>
       </c>
       <c r="C5">
-        <v>61.499600000000001</v>
+        <v>61.4996</v>
       </c>
       <c r="D5">
-        <v>7.8422000000000001</v>
+        <v>7.8422</v>
       </c>
       <c r="E5">
-        <v>0.93259999999999998</v>
+        <v>0.9326</v>
       </c>
       <c r="F5">
         <v>0.1865</v>
       </c>
       <c r="G5">
-        <v>0.13800000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.7863000000000002</v>
+        <v>3.7863</v>
       </c>
       <c r="C6">
-        <v>26.417899999999999</v>
+        <v>26.4179</v>
       </c>
       <c r="D6">
-        <v>5.1398000000000001</v>
+        <v>5.1398</v>
       </c>
       <c r="E6">
-        <v>0.95979999999999999</v>
+        <v>0.9598</v>
       </c>
       <c r="F6">
-        <v>0.10059999999999999</v>
+        <v>0.1006</v>
       </c>
       <c r="G6">
-        <v>7.1599999999999997E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5974000000000004</v>
+        <v>4.5974</v>
       </c>
       <c r="C7">
-        <v>39.789499999999997</v>
+        <v>39.7895</v>
       </c>
       <c r="D7">
         <v>6.1574</v>
       </c>
       <c r="E7">
-        <v>0.94750000000000001</v>
+        <v>0.9475</v>
       </c>
       <c r="F7">
         <v>0.1106</v>
       </c>
       <c r="G7">
-        <v>8.48E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.0848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.81369999999999998</v>
+        <v>0.8137</v>
       </c>
       <c r="C8">
-        <v>17.594899999999999</v>
+        <v>17.5949</v>
       </c>
       <c r="D8">
-        <v>1.3698999999999999</v>
+        <v>1.3699</v>
       </c>
       <c r="E8">
-        <v>2.12E-2</v>
+        <v>0.0212</v>
       </c>
       <c r="F8">
-        <v>4.1000000000000002E-2</v>
+        <v>0.041</v>
       </c>
       <c r="G8">
-        <v>2.81E-2</v>
+        <v>0.0281</v>
       </c>
     </row>
   </sheetData>
@@ -2656,14 +2591,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2694,22 +2629,22 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>4.5871000000000004</v>
+        <v>4.5871</v>
       </c>
       <c r="D2">
-        <v>34.286200000000001</v>
+        <v>34.2862</v>
       </c>
       <c r="E2">
-        <v>5.8554000000000004</v>
+        <v>5.8554</v>
       </c>
       <c r="F2">
-        <v>0.93079999999999996</v>
+        <v>0.9308</v>
       </c>
       <c r="G2">
-        <v>9.2999999999999999E-2</v>
+        <v>0.093</v>
       </c>
       <c r="H2">
-        <v>7.7299999999999994E-2</v>
+        <v>0.07729999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update modeling notebook to improve final plot (xlim, grid, etc.)
</commit_message>
<xml_diff>
--- a/models/regression_model_1m/pycaret_tables.xlsx
+++ b/models/regression_model_1m/pycaret_tables.xlsx
@@ -50,33 +50,33 @@
     <t>TT (Sec)</t>
   </si>
   <si>
+    <t>gbr</t>
+  </si>
+  <si>
     <t>et</t>
   </si>
   <si>
-    <t>gbr</t>
-  </si>
-  <si>
     <t>lightgbm</t>
   </si>
   <si>
     <t>rf</t>
   </si>
   <si>
+    <t>ada</t>
+  </si>
+  <si>
     <t>lr</t>
   </si>
   <si>
-    <t>ada</t>
+    <t>ridge</t>
+  </si>
+  <si>
+    <t>br</t>
   </si>
   <si>
     <t>huber</t>
   </si>
   <si>
-    <t>ridge</t>
-  </si>
-  <si>
-    <t>br</t>
-  </si>
-  <si>
     <t>lasso</t>
   </si>
   <si>
@@ -86,12 +86,12 @@
     <t>omp</t>
   </si>
   <si>
+    <t>dt</t>
+  </si>
+  <si>
     <t>en</t>
   </si>
   <si>
-    <t>dt</t>
-  </si>
-  <si>
     <t>par</t>
   </si>
   <si>
@@ -104,33 +104,33 @@
     <t>lar</t>
   </si>
   <si>
+    <t>Gradient Boosting Regressor</t>
+  </si>
+  <si>
     <t>Extra Trees Regressor</t>
   </si>
   <si>
-    <t>Gradient Boosting Regressor</t>
-  </si>
-  <si>
     <t>Light Gradient Boosting Machine</t>
   </si>
   <si>
     <t>Random Forest Regressor</t>
   </si>
   <si>
+    <t>AdaBoost Regressor</t>
+  </si>
+  <si>
     <t>Linear Regression</t>
   </si>
   <si>
-    <t>AdaBoost Regressor</t>
+    <t>Ridge Regression</t>
+  </si>
+  <si>
+    <t>Bayesian Ridge</t>
   </si>
   <si>
     <t>Huber Regressor</t>
   </si>
   <si>
-    <t>Ridge Regression</t>
-  </si>
-  <si>
-    <t>Bayesian Ridge</t>
-  </si>
-  <si>
     <t>Lasso Regression</t>
   </si>
   <si>
@@ -140,10 +140,10 @@
     <t>Orthogonal Matching Pursuit</t>
   </si>
   <si>
+    <t>Decision Tree Regressor</t>
+  </si>
+  <si>
     <t>Elastic Net</t>
-  </si>
-  <si>
-    <t>Decision Tree Regressor</t>
   </si>
   <si>
     <t>Passive Aggressive Regressor</t>
@@ -568,25 +568,25 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>4.5075</v>
+        <v>4.6119</v>
       </c>
       <c r="D2">
-        <v>40.471</v>
+        <v>42.6163</v>
       </c>
       <c r="E2">
-        <v>6.315</v>
+        <v>6.3519</v>
       </c>
       <c r="F2">
-        <v>0.946</v>
+        <v>0.9407</v>
       </c>
       <c r="G2">
-        <v>0.115</v>
+        <v>0.1131</v>
       </c>
       <c r="H2">
-        <v>0.08450000000000001</v>
+        <v>0.0847</v>
       </c>
       <c r="I2">
-        <v>0.074</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -597,25 +597,25 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>5.1025</v>
+        <v>4.4981</v>
       </c>
       <c r="D3">
-        <v>48.2418</v>
+        <v>44.6487</v>
       </c>
       <c r="E3">
-        <v>6.8486</v>
+        <v>6.458</v>
       </c>
       <c r="F3">
-        <v>0.9354</v>
+        <v>0.9384</v>
       </c>
       <c r="G3">
-        <v>0.1201</v>
+        <v>0.1131</v>
       </c>
       <c r="H3">
-        <v>0.0924</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="I3">
-        <v>0.054</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -626,25 +626,25 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <v>5.2173</v>
+        <v>4.8927</v>
       </c>
       <c r="D4">
-        <v>53.3653</v>
+        <v>45.0184</v>
       </c>
       <c r="E4">
-        <v>7.2457</v>
+        <v>6.5788</v>
       </c>
       <c r="F4">
-        <v>0.9288999999999999</v>
+        <v>0.9377</v>
       </c>
       <c r="G4">
-        <v>0.1223</v>
+        <v>0.1174</v>
       </c>
       <c r="H4">
-        <v>0.09329999999999999</v>
+        <v>0.0914</v>
       </c>
       <c r="I4">
-        <v>0.036</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -655,25 +655,25 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>5.2954</v>
+        <v>4.8434</v>
       </c>
       <c r="D5">
-        <v>55.0556</v>
+        <v>46.3525</v>
       </c>
       <c r="E5">
-        <v>7.3763</v>
+        <v>6.6849</v>
       </c>
       <c r="F5">
-        <v>0.9261</v>
+        <v>0.9361</v>
       </c>
       <c r="G5">
-        <v>0.1299</v>
+        <v>0.1174</v>
       </c>
       <c r="H5">
-        <v>0.09619999999999999</v>
+        <v>0.0892</v>
       </c>
       <c r="I5">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -684,25 +684,25 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>5.8957</v>
+        <v>5.4859</v>
       </c>
       <c r="D6">
-        <v>56.6823</v>
+        <v>52.53</v>
       </c>
       <c r="E6">
-        <v>7.4881</v>
+        <v>7.1626</v>
       </c>
       <c r="F6">
-        <v>0.9252</v>
+        <v>0.9276</v>
       </c>
       <c r="G6">
-        <v>0.1551</v>
+        <v>0.1289</v>
       </c>
       <c r="H6">
-        <v>0.118</v>
+        <v>0.1033</v>
       </c>
       <c r="I6">
-        <v>1.146</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -713,25 +713,25 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>5.7991</v>
+        <v>5.8856</v>
       </c>
       <c r="D7">
-        <v>59.5745</v>
+        <v>58.3605</v>
       </c>
       <c r="E7">
-        <v>7.6263</v>
+        <v>7.5929</v>
       </c>
       <c r="F7">
         <v>0.9205</v>
       </c>
       <c r="G7">
-        <v>0.1333</v>
+        <v>0.1659</v>
       </c>
       <c r="H7">
-        <v>0.1076</v>
+        <v>0.1191</v>
       </c>
       <c r="I7">
-        <v>0.052</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -742,25 +742,25 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>5.8054</v>
+        <v>5.9879</v>
       </c>
       <c r="D8">
-        <v>58.8903</v>
+        <v>58.5232</v>
       </c>
       <c r="E8">
-        <v>7.6361</v>
+        <v>7.6147</v>
       </c>
       <c r="F8">
-        <v>0.9222</v>
+        <v>0.9204</v>
       </c>
       <c r="G8">
-        <v>0.1569</v>
+        <v>0.163</v>
       </c>
       <c r="H8">
-        <v>0.1162</v>
+        <v>0.1188</v>
       </c>
       <c r="I8">
-        <v>0.026</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -771,25 +771,25 @@
         <v>33</v>
       </c>
       <c r="C9">
-        <v>5.9442</v>
+        <v>6.0679</v>
       </c>
       <c r="D9">
-        <v>59.6758</v>
+        <v>60.2652</v>
       </c>
       <c r="E9">
-        <v>7.6896</v>
+        <v>7.726</v>
       </c>
       <c r="F9">
-        <v>0.9207</v>
+        <v>0.9182</v>
       </c>
       <c r="G9">
-        <v>0.155</v>
+        <v>0.1671</v>
       </c>
       <c r="H9">
-        <v>0.1166</v>
+        <v>0.1208</v>
       </c>
       <c r="I9">
-        <v>0.028</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -800,25 +800,25 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>6.0204</v>
+        <v>6.2296</v>
       </c>
       <c r="D10">
-        <v>62.5989</v>
+        <v>65.2736</v>
       </c>
       <c r="E10">
-        <v>7.8761</v>
+        <v>8.0244</v>
       </c>
       <c r="F10">
-        <v>0.9165</v>
+        <v>0.9112</v>
       </c>
       <c r="G10">
-        <v>0.1584</v>
+        <v>0.1705</v>
       </c>
       <c r="H10">
-        <v>0.1173</v>
+        <v>0.1244</v>
       </c>
       <c r="I10">
-        <v>0.02</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -829,25 +829,25 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>6.2585</v>
+        <v>6.2749</v>
       </c>
       <c r="D11">
-        <v>68.0508</v>
+        <v>68.5926</v>
       </c>
       <c r="E11">
-        <v>8.217499999999999</v>
+        <v>8.209300000000001</v>
       </c>
       <c r="F11">
-        <v>0.9094</v>
+        <v>0.9074</v>
       </c>
       <c r="G11">
-        <v>0.1603</v>
+        <v>0.1594</v>
       </c>
       <c r="H11">
-        <v>0.1227</v>
+        <v>0.1226</v>
       </c>
       <c r="I11">
-        <v>0.578</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -858,25 +858,25 @@
         <v>36</v>
       </c>
       <c r="C12">
-        <v>5.8895</v>
+        <v>5.8394</v>
       </c>
       <c r="D12">
-        <v>73.73650000000001</v>
+        <v>76.0692</v>
       </c>
       <c r="E12">
-        <v>8.423999999999999</v>
+        <v>8.6463</v>
       </c>
       <c r="F12">
-        <v>0.9046999999999999</v>
+        <v>0.8983</v>
       </c>
       <c r="G12">
-        <v>0.1415</v>
+        <v>0.1417</v>
       </c>
       <c r="H12">
-        <v>0.1092</v>
+        <v>0.106</v>
       </c>
       <c r="I12">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -887,25 +887,25 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>6.3058</v>
+        <v>6.5508</v>
       </c>
       <c r="D13">
-        <v>75.9007</v>
+        <v>78.0218</v>
       </c>
       <c r="E13">
-        <v>8.695600000000001</v>
+        <v>8.751099999999999</v>
       </c>
       <c r="F13">
-        <v>0.8972</v>
+        <v>0.8944</v>
       </c>
       <c r="G13">
-        <v>0.1697</v>
+        <v>0.174</v>
       </c>
       <c r="H13">
-        <v>0.1241</v>
+        <v>0.1275</v>
       </c>
       <c r="I13">
-        <v>0.024</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -916,25 +916,25 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>6.8563</v>
+        <v>6.3379</v>
       </c>
       <c r="D14">
-        <v>79.071</v>
+        <v>82.4756</v>
       </c>
       <c r="E14">
-        <v>8.8599</v>
+        <v>8.9153</v>
       </c>
       <c r="F14">
-        <v>0.8949</v>
+        <v>0.8858</v>
       </c>
       <c r="G14">
-        <v>0.1657</v>
+        <v>0.1484</v>
       </c>
       <c r="H14">
-        <v>0.1325</v>
+        <v>0.1107</v>
       </c>
       <c r="I14">
-        <v>0.022</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -945,22 +945,22 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>6.6427</v>
+        <v>6.9746</v>
       </c>
       <c r="D15">
-        <v>84.36839999999999</v>
+        <v>82.6238</v>
       </c>
       <c r="E15">
-        <v>9.0702</v>
+        <v>9.057399999999999</v>
       </c>
       <c r="F15">
-        <v>0.8842</v>
+        <v>0.8883</v>
       </c>
       <c r="G15">
-        <v>0.1536</v>
+        <v>0.1659</v>
       </c>
       <c r="H15">
-        <v>0.1183</v>
+        <v>0.1332</v>
       </c>
       <c r="I15">
         <v>0.018</v>
@@ -974,25 +974,25 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>8.6614</v>
+        <v>7.4808</v>
       </c>
       <c r="D16">
-        <v>132.6311</v>
+        <v>94.4228</v>
       </c>
       <c r="E16">
-        <v>10.8966</v>
+        <v>9.523</v>
       </c>
       <c r="F16">
-        <v>0.8177</v>
+        <v>0.8731</v>
       </c>
       <c r="G16">
-        <v>0.3149</v>
+        <v>0.2444</v>
       </c>
       <c r="H16">
-        <v>0.1884</v>
+        <v>0.1519</v>
       </c>
       <c r="I16">
-        <v>0.022</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1003,25 +1003,25 @@
         <v>41</v>
       </c>
       <c r="C17">
-        <v>12.8847</v>
+        <v>13.0727</v>
       </c>
       <c r="D17">
-        <v>249.6969</v>
+        <v>245.198</v>
       </c>
       <c r="E17">
-        <v>15.7637</v>
+        <v>15.6182</v>
       </c>
       <c r="F17">
-        <v>0.6677</v>
+        <v>0.6698</v>
       </c>
       <c r="G17">
-        <v>0.2795</v>
+        <v>0.2858</v>
       </c>
       <c r="H17">
-        <v>0.2643</v>
+        <v>0.2712</v>
       </c>
       <c r="I17">
-        <v>0.02</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1032,25 +1032,25 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>23.2068</v>
+        <v>23.5358</v>
       </c>
       <c r="D18">
-        <v>756.9346</v>
+        <v>751.4456</v>
       </c>
       <c r="E18">
-        <v>27.4508</v>
+        <v>27.3783</v>
       </c>
       <c r="F18">
-        <v>-0.0056</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="G18">
-        <v>0.4782</v>
+        <v>0.4839</v>
       </c>
       <c r="H18">
-        <v>0.4956</v>
+        <v>0.5058</v>
       </c>
       <c r="I18">
-        <v>0.026</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1061,25 +1061,25 @@
         <v>43</v>
       </c>
       <c r="C19">
-        <v>4382.0176</v>
+        <v>111.3592</v>
       </c>
       <c r="D19">
-        <v>192874824.186</v>
+        <v>55904.4646</v>
       </c>
       <c r="E19">
-        <v>6358.1619</v>
+        <v>153.1446</v>
       </c>
       <c r="F19">
-        <v>-272295.7716</v>
+        <v>-76.3618</v>
       </c>
       <c r="G19">
-        <v>1.8959</v>
+        <v>1.0019</v>
       </c>
       <c r="H19">
-        <v>75.4915</v>
+        <v>1.9531</v>
       </c>
       <c r="I19">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -1126,22 +1126,22 @@
         <v>48</v>
       </c>
       <c r="C2">
-        <v>5.2775</v>
+        <v>4.9824</v>
       </c>
       <c r="D2">
-        <v>44.2081</v>
+        <v>36.2245</v>
       </c>
       <c r="E2">
-        <v>6.6489</v>
+        <v>6.0187</v>
       </c>
       <c r="F2">
-        <v>0.9107</v>
+        <v>0.9263</v>
       </c>
       <c r="G2">
-        <v>0.1042</v>
+        <v>0.098</v>
       </c>
       <c r="H2">
-        <v>0.0881</v>
+        <v>0.0825</v>
       </c>
     </row>
   </sheetData>
@@ -1185,25 +1185,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2">
-        <v>0.9828</v>
+        <v>2.6303</v>
       </c>
       <c r="D2">
-        <v>1.9863</v>
+        <v>10.763</v>
       </c>
       <c r="E2">
-        <v>1.4094</v>
+        <v>3.2807</v>
       </c>
       <c r="F2">
-        <v>0.9971</v>
+        <v>0.9781</v>
       </c>
       <c r="G2">
-        <v>0.0246</v>
+        <v>0.0521</v>
       </c>
       <c r="H2">
-        <v>0.0164</v>
+        <v>0.0437</v>
       </c>
     </row>
   </sheetData>
@@ -1247,22 +1247,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.4767</v>
+        <v>3.7133</v>
       </c>
       <c r="C2">
-        <v>35.6244</v>
+        <v>24.4168</v>
       </c>
       <c r="D2">
-        <v>5.9686</v>
+        <v>4.9413</v>
       </c>
       <c r="E2">
-        <v>0.9567</v>
+        <v>0.9664</v>
       </c>
       <c r="F2">
-        <v>0.0804</v>
+        <v>0.0733</v>
       </c>
       <c r="G2">
-        <v>0.06759999999999999</v>
+        <v>0.0585</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1270,22 +1270,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.6016</v>
+        <v>3.9891</v>
       </c>
       <c r="C3">
-        <v>36.6182</v>
+        <v>29.7275</v>
       </c>
       <c r="D3">
-        <v>6.0513</v>
+        <v>5.4523</v>
       </c>
       <c r="E3">
-        <v>0.9483</v>
+        <v>0.9636</v>
       </c>
       <c r="F3">
-        <v>0.08890000000000001</v>
+        <v>0.078</v>
       </c>
       <c r="G3">
-        <v>0.06</v>
+        <v>0.0654</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1293,22 +1293,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.3482</v>
+        <v>4.2799</v>
       </c>
       <c r="C4">
-        <v>31.7973</v>
+        <v>35.5947</v>
       </c>
       <c r="D4">
-        <v>5.6389</v>
+        <v>5.9661</v>
       </c>
       <c r="E4">
-        <v>0.952</v>
+        <v>0.9435</v>
       </c>
       <c r="F4">
-        <v>0.0844</v>
+        <v>0.09370000000000001</v>
       </c>
       <c r="G4">
-        <v>0.0722</v>
+        <v>0.0706</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1316,22 +1316,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.447</v>
+        <v>3.4232</v>
       </c>
       <c r="C5">
-        <v>80.9879</v>
+        <v>17.9163</v>
       </c>
       <c r="D5">
-        <v>8.9993</v>
+        <v>4.2328</v>
       </c>
       <c r="E5">
-        <v>0.9112</v>
+        <v>0.9782999999999999</v>
       </c>
       <c r="F5">
-        <v>0.2168</v>
+        <v>0.0775</v>
       </c>
       <c r="G5">
-        <v>0.1636</v>
+        <v>0.0639</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1339,22 +1339,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.2917</v>
+        <v>5.8833</v>
       </c>
       <c r="C6">
-        <v>38.2074</v>
+        <v>69.8308</v>
       </c>
       <c r="D6">
-        <v>6.1812</v>
+        <v>8.3565</v>
       </c>
       <c r="E6">
-        <v>0.9419</v>
+        <v>0.9035</v>
       </c>
       <c r="F6">
-        <v>0.115</v>
+        <v>0.1901</v>
       </c>
       <c r="G6">
-        <v>0.081</v>
+        <v>0.1336</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1362,22 +1362,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.633</v>
+        <v>4.2578</v>
       </c>
       <c r="C7">
-        <v>44.647</v>
+        <v>35.4972</v>
       </c>
       <c r="D7">
-        <v>6.5679</v>
+        <v>5.7898</v>
       </c>
       <c r="E7">
-        <v>0.9419999999999999</v>
+        <v>0.9510999999999999</v>
       </c>
       <c r="F7">
-        <v>0.1171</v>
+        <v>0.1025</v>
       </c>
       <c r="G7">
-        <v>0.08890000000000001</v>
+        <v>0.0784</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1385,22 +1385,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.9567</v>
+        <v>0.8612</v>
       </c>
       <c r="C8">
-        <v>18.2927</v>
+        <v>18.1326</v>
       </c>
       <c r="D8">
-        <v>1.2289</v>
+        <v>1.4055</v>
       </c>
       <c r="E8">
-        <v>0.0162</v>
+        <v>0.0263</v>
       </c>
       <c r="F8">
-        <v>0.0513</v>
+        <v>0.0443</v>
       </c>
       <c r="G8">
-        <v>0.038</v>
+        <v>0.0279</v>
       </c>
     </row>
   </sheetData>
@@ -1444,22 +1444,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.6779</v>
+        <v>4.2013</v>
       </c>
       <c r="C2">
-        <v>34.3328</v>
+        <v>34.5914</v>
       </c>
       <c r="D2">
-        <v>5.8594</v>
+        <v>5.8814</v>
       </c>
       <c r="E2">
-        <v>0.9582000000000001</v>
+        <v>0.9524</v>
       </c>
       <c r="F2">
-        <v>0.0887</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="G2">
-        <v>0.0733</v>
+        <v>0.0673</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1467,22 +1467,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.3189</v>
+        <v>4.1276</v>
       </c>
       <c r="C3">
-        <v>59.4736</v>
+        <v>33.1818</v>
       </c>
       <c r="D3">
-        <v>7.7119</v>
+        <v>5.7604</v>
       </c>
       <c r="E3">
-        <v>0.916</v>
+        <v>0.9594</v>
       </c>
       <c r="F3">
-        <v>0.1146</v>
+        <v>0.0922</v>
       </c>
       <c r="G3">
-        <v>0.0891</v>
+        <v>0.07240000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1490,22 +1490,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.875</v>
+        <v>3.9935</v>
       </c>
       <c r="C4">
-        <v>23.571</v>
+        <v>34.371</v>
       </c>
       <c r="D4">
-        <v>4.855</v>
+        <v>5.8627</v>
       </c>
       <c r="E4">
-        <v>0.9644</v>
+        <v>0.9454</v>
       </c>
       <c r="F4">
-        <v>0.0919</v>
+        <v>0.0907</v>
       </c>
       <c r="G4">
-        <v>0.0699</v>
+        <v>0.0665</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1513,22 +1513,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.5547</v>
+        <v>3.9575</v>
       </c>
       <c r="C5">
-        <v>57.3705</v>
+        <v>23.6778</v>
       </c>
       <c r="D5">
-        <v>7.5743</v>
+        <v>4.866</v>
       </c>
       <c r="E5">
-        <v>0.9371</v>
+        <v>0.9713000000000001</v>
       </c>
       <c r="F5">
-        <v>0.188</v>
+        <v>0.0883</v>
       </c>
       <c r="G5">
-        <v>0.1366</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1536,22 +1536,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.3128</v>
+        <v>6.3447</v>
       </c>
       <c r="C6">
-        <v>20.7651</v>
+        <v>91</v>
       </c>
       <c r="D6">
-        <v>4.5569</v>
+        <v>9.539400000000001</v>
       </c>
       <c r="E6">
-        <v>0.9684</v>
+        <v>0.8743</v>
       </c>
       <c r="F6">
-        <v>0.08840000000000001</v>
+        <v>0.1946</v>
       </c>
       <c r="G6">
-        <v>0.0626</v>
+        <v>0.1417</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1559,22 +1559,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5479</v>
+        <v>4.5249</v>
       </c>
       <c r="C7">
-        <v>39.1026</v>
+        <v>43.3644</v>
       </c>
       <c r="D7">
-        <v>6.1115</v>
+        <v>6.382</v>
       </c>
       <c r="E7">
-        <v>0.9488</v>
+        <v>0.9406</v>
       </c>
       <c r="F7">
-        <v>0.1143</v>
+        <v>0.1113</v>
       </c>
       <c r="G7">
-        <v>0.0863</v>
+        <v>0.0844</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1582,22 +1582,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.8489</v>
+        <v>0.9142</v>
       </c>
       <c r="C8">
-        <v>16.4252</v>
+        <v>24.1588</v>
       </c>
       <c r="D8">
-        <v>1.3237</v>
+        <v>1.6232</v>
       </c>
       <c r="E8">
-        <v>0.0196</v>
+        <v>0.0342</v>
       </c>
       <c r="F8">
-        <v>0.0381</v>
+        <v>0.0417</v>
       </c>
       <c r="G8">
-        <v>0.0266</v>
+        <v>0.0288</v>
       </c>
     </row>
   </sheetData>
@@ -1641,22 +1641,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.0395</v>
+        <v>4.6571</v>
       </c>
       <c r="C2">
-        <v>45.9624</v>
+        <v>33.542</v>
       </c>
       <c r="D2">
-        <v>6.7796</v>
+        <v>5.7915</v>
       </c>
       <c r="E2">
-        <v>0.9441000000000001</v>
+        <v>0.9539</v>
       </c>
       <c r="F2">
-        <v>0.0968</v>
+        <v>0.1039</v>
       </c>
       <c r="G2">
-        <v>0.0765</v>
+        <v>0.08119999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1664,22 +1664,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.2368</v>
+        <v>3.9068</v>
       </c>
       <c r="C3">
-        <v>63.5893</v>
+        <v>24.7167</v>
       </c>
       <c r="D3">
-        <v>7.9743</v>
+        <v>4.9716</v>
       </c>
       <c r="E3">
-        <v>0.9102</v>
+        <v>0.9698</v>
       </c>
       <c r="F3">
-        <v>0.1152</v>
+        <v>0.0837</v>
       </c>
       <c r="G3">
-        <v>0.0867</v>
+        <v>0.0699</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1687,22 +1687,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.6568</v>
+        <v>4.6063</v>
       </c>
       <c r="C4">
-        <v>32.5161</v>
+        <v>34.9543</v>
       </c>
       <c r="D4">
-        <v>5.7023</v>
+        <v>5.9122</v>
       </c>
       <c r="E4">
-        <v>0.9509</v>
+        <v>0.9445</v>
       </c>
       <c r="F4">
-        <v>0.1029</v>
+        <v>0.1003</v>
       </c>
       <c r="G4">
-        <v>0.079</v>
+        <v>0.0809</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1710,22 +1710,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.6617</v>
+        <v>3.9057</v>
       </c>
       <c r="C5">
-        <v>57.0659</v>
+        <v>22.8745</v>
       </c>
       <c r="D5">
-        <v>7.5542</v>
+        <v>4.7827</v>
       </c>
       <c r="E5">
-        <v>0.9374</v>
+        <v>0.9723000000000001</v>
       </c>
       <c r="F5">
-        <v>0.1773</v>
+        <v>0.08690000000000001</v>
       </c>
       <c r="G5">
-        <v>0.134</v>
+        <v>0.07240000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1733,22 +1733,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5.0891</v>
+        <v>6.7308</v>
       </c>
       <c r="C6">
-        <v>46.3525</v>
+        <v>78.815</v>
       </c>
       <c r="D6">
-        <v>6.8083</v>
+        <v>8.877800000000001</v>
       </c>
       <c r="E6">
-        <v>0.9295</v>
+        <v>0.8911</v>
       </c>
       <c r="F6">
-        <v>0.1196</v>
+        <v>0.1909</v>
       </c>
       <c r="G6">
-        <v>0.0911</v>
+        <v>0.1469</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1756,22 +1756,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>5.1368</v>
+        <v>4.7613</v>
       </c>
       <c r="C7">
-        <v>49.0972</v>
+        <v>38.9805</v>
       </c>
       <c r="D7">
-        <v>6.9637</v>
+        <v>6.0672</v>
       </c>
       <c r="E7">
-        <v>0.9344</v>
+        <v>0.9463</v>
       </c>
       <c r="F7">
-        <v>0.1224</v>
+        <v>0.1131</v>
       </c>
       <c r="G7">
-        <v>0.0935</v>
+        <v>0.09030000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1779,22 +1779,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.3248</v>
+        <v>1.0369</v>
       </c>
       <c r="C8">
-        <v>10.6378</v>
+        <v>20.4716</v>
       </c>
       <c r="D8">
-        <v>0.7771</v>
+        <v>1.4731</v>
       </c>
       <c r="E8">
-        <v>0.014</v>
+        <v>0.0294</v>
       </c>
       <c r="F8">
+        <v>0.0396</v>
+      </c>
+      <c r="G8">
         <v>0.0287</v>
-      </c>
-      <c r="G8">
-        <v>0.0209</v>
       </c>
     </row>
   </sheetData>
@@ -1838,22 +1838,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.8397</v>
+        <v>4.1175</v>
       </c>
       <c r="C2">
-        <v>41.2268</v>
+        <v>33.9625</v>
       </c>
       <c r="D2">
-        <v>6.4208</v>
+        <v>5.8277</v>
       </c>
       <c r="E2">
-        <v>0.9498</v>
+        <v>0.9533</v>
       </c>
       <c r="F2">
-        <v>0.08840000000000001</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="G2">
-        <v>0.07290000000000001</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1861,22 +1861,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.7935</v>
+        <v>4.4045</v>
       </c>
       <c r="C3">
-        <v>52.8236</v>
+        <v>39.9219</v>
       </c>
       <c r="D3">
-        <v>7.268</v>
+        <v>6.3184</v>
       </c>
       <c r="E3">
-        <v>0.9254</v>
+        <v>0.9512</v>
       </c>
       <c r="F3">
-        <v>0.1071</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="G3">
-        <v>0.0774</v>
+        <v>0.0737</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1884,22 +1884,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2358</v>
+        <v>4.6193</v>
       </c>
       <c r="C4">
-        <v>27.6849</v>
+        <v>39.3926</v>
       </c>
       <c r="D4">
-        <v>5.2616</v>
+        <v>6.2764</v>
       </c>
       <c r="E4">
-        <v>0.9582000000000001</v>
+        <v>0.9374</v>
       </c>
       <c r="F4">
-        <v>0.0891</v>
+        <v>0.1003</v>
       </c>
       <c r="G4">
-        <v>0.0741</v>
+        <v>0.0771</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1907,22 +1907,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.7356</v>
+        <v>3.868</v>
       </c>
       <c r="C5">
-        <v>60.7155</v>
+        <v>23.516</v>
       </c>
       <c r="D5">
-        <v>7.792</v>
+        <v>4.8493</v>
       </c>
       <c r="E5">
-        <v>0.9334</v>
+        <v>0.9715</v>
       </c>
       <c r="F5">
-        <v>0.1975</v>
+        <v>0.0907</v>
       </c>
       <c r="G5">
-        <v>0.1446</v>
+        <v>0.0735</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1930,22 +1930,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.0213</v>
+        <v>6.1452</v>
       </c>
       <c r="C6">
-        <v>32.0038</v>
+        <v>79.563</v>
       </c>
       <c r="D6">
-        <v>5.6572</v>
+        <v>8.9198</v>
       </c>
       <c r="E6">
-        <v>0.9513</v>
+        <v>0.8901</v>
       </c>
       <c r="F6">
-        <v>0.1077</v>
+        <v>0.1997</v>
       </c>
       <c r="G6">
-        <v>0.07630000000000001</v>
+        <v>0.1426</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1953,22 +1953,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.7252</v>
+        <v>4.6309</v>
       </c>
       <c r="C7">
-        <v>42.8909</v>
+        <v>43.2712</v>
       </c>
       <c r="D7">
-        <v>6.4799</v>
+        <v>6.4383</v>
       </c>
       <c r="E7">
-        <v>0.9436</v>
+        <v>0.9407</v>
       </c>
       <c r="F7">
-        <v>0.118</v>
+        <v>0.1144</v>
       </c>
       <c r="G7">
-        <v>0.0891</v>
+        <v>0.0868</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1976,22 +1976,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.5956</v>
+        <v>0.7988</v>
       </c>
       <c r="C8">
-        <v>12.4008</v>
+        <v>19.0802</v>
       </c>
       <c r="D8">
-        <v>0.9494</v>
+        <v>1.3488</v>
       </c>
       <c r="E8">
-        <v>0.0122</v>
+        <v>0.0275</v>
       </c>
       <c r="F8">
-        <v>0.0406</v>
+        <v>0.0429</v>
       </c>
       <c r="G8">
-        <v>0.0278</v>
+        <v>0.0281</v>
       </c>
     </row>
   </sheetData>
@@ -2035,22 +2035,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6.7322</v>
+        <v>5.2691</v>
       </c>
       <c r="C2">
-        <v>67.2937</v>
+        <v>50.2971</v>
       </c>
       <c r="D2">
-        <v>8.2033</v>
+        <v>7.092</v>
       </c>
       <c r="E2">
-        <v>0.9181</v>
+        <v>0.9308</v>
       </c>
       <c r="F2">
-        <v>0.1426</v>
+        <v>0.1152</v>
       </c>
       <c r="G2">
-        <v>0.1131</v>
+        <v>0.09089999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2058,22 +2058,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.1848</v>
+        <v>4.9616</v>
       </c>
       <c r="C3">
-        <v>49.8998</v>
+        <v>43.6126</v>
       </c>
       <c r="D3">
-        <v>7.064</v>
+        <v>6.604</v>
       </c>
       <c r="E3">
-        <v>0.9295</v>
+        <v>0.9467</v>
       </c>
       <c r="F3">
-        <v>0.1604</v>
+        <v>0.1034</v>
       </c>
       <c r="G3">
-        <v>0.1058</v>
+        <v>0.0857</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2081,22 +2081,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6.0945</v>
+        <v>5.7887</v>
       </c>
       <c r="C4">
-        <v>53.8813</v>
+        <v>54.1168</v>
       </c>
       <c r="D4">
-        <v>7.3404</v>
+        <v>7.3564</v>
       </c>
       <c r="E4">
-        <v>0.9186</v>
+        <v>0.914</v>
       </c>
       <c r="F4">
-        <v>0.1291</v>
+        <v>0.1164</v>
       </c>
       <c r="G4">
-        <v>0.1077</v>
+        <v>0.0969</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2104,22 +2104,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.5391</v>
+        <v>5.2472</v>
       </c>
       <c r="C5">
-        <v>72.1733</v>
+        <v>37.3582</v>
       </c>
       <c r="D5">
-        <v>8.4955</v>
+        <v>6.1121</v>
       </c>
       <c r="E5">
-        <v>0.9208</v>
+        <v>0.9547</v>
       </c>
       <c r="F5">
-        <v>0.2117</v>
+        <v>0.1176</v>
       </c>
       <c r="G5">
-        <v>0.161</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2127,22 +2127,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.9277</v>
+        <v>6.5108</v>
       </c>
       <c r="C6">
-        <v>40.1634</v>
+        <v>80.4537</v>
       </c>
       <c r="D6">
-        <v>6.3375</v>
+        <v>8.9696</v>
       </c>
       <c r="E6">
-        <v>0.9389</v>
+        <v>0.8888</v>
       </c>
       <c r="F6">
-        <v>0.132</v>
+        <v>0.2017</v>
       </c>
       <c r="G6">
-        <v>0.1022</v>
+        <v>0.1522</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2150,22 +2150,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>5.8957</v>
+        <v>5.5555</v>
       </c>
       <c r="C7">
-        <v>56.6823</v>
+        <v>53.1677</v>
       </c>
       <c r="D7">
-        <v>7.4881</v>
+        <v>7.2268</v>
       </c>
       <c r="E7">
-        <v>0.9252</v>
+        <v>0.927</v>
       </c>
       <c r="F7">
-        <v>0.1551</v>
+        <v>0.1308</v>
       </c>
       <c r="G7">
-        <v>0.118</v>
+        <v>0.1053</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2173,22 +2173,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.7205</v>
+        <v>0.5471</v>
       </c>
       <c r="C8">
-        <v>11.6559</v>
+        <v>14.798</v>
       </c>
       <c r="D8">
-        <v>0.7813</v>
+        <v>0.9698</v>
       </c>
       <c r="E8">
-        <v>0.008</v>
+        <v>0.0236</v>
       </c>
       <c r="F8">
-        <v>0.0303</v>
+        <v>0.0358</v>
       </c>
       <c r="G8">
-        <v>0.0218</v>
+        <v>0.024</v>
       </c>
     </row>
   </sheetData>
@@ -2232,22 +2232,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.7849</v>
+        <v>4.127</v>
       </c>
       <c r="C2">
-        <v>36.0137</v>
+        <v>31.3801</v>
       </c>
       <c r="D2">
-        <v>6.0011</v>
+        <v>5.6018</v>
       </c>
       <c r="E2">
-        <v>0.9562</v>
+        <v>0.9569</v>
       </c>
       <c r="F2">
-        <v>0.0872</v>
+        <v>0.0858</v>
       </c>
       <c r="G2">
-        <v>0.0736</v>
+        <v>0.0663</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2255,22 +2255,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.4661</v>
+        <v>4.0218</v>
       </c>
       <c r="C3">
-        <v>47.8932</v>
+        <v>29.6332</v>
       </c>
       <c r="D3">
-        <v>6.9205</v>
+        <v>5.4436</v>
       </c>
       <c r="E3">
-        <v>0.9324</v>
+        <v>0.9638</v>
       </c>
       <c r="F3">
-        <v>0.1016</v>
+        <v>0.08169999999999999</v>
       </c>
       <c r="G3">
-        <v>0.0757</v>
+        <v>0.06759999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2278,22 +2278,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.3926</v>
+        <v>4.2125</v>
       </c>
       <c r="C4">
-        <v>28.0386</v>
+        <v>33.6663</v>
       </c>
       <c r="D4">
-        <v>5.2951</v>
+        <v>5.8023</v>
       </c>
       <c r="E4">
-        <v>0.9577</v>
+        <v>0.9465</v>
       </c>
       <c r="F4">
-        <v>0.09080000000000001</v>
+        <v>0.0924</v>
       </c>
       <c r="G4">
-        <v>0.0752</v>
+        <v>0.0707</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2301,22 +2301,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.4943</v>
+        <v>3.7362</v>
       </c>
       <c r="C5">
-        <v>53.3835</v>
+        <v>19.663</v>
       </c>
       <c r="D5">
-        <v>7.3064</v>
+        <v>4.4343</v>
       </c>
       <c r="E5">
-        <v>0.9415</v>
+        <v>0.9762</v>
       </c>
       <c r="F5">
-        <v>0.1802</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="G5">
-        <v>0.1332</v>
+        <v>0.0703</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2324,22 +2324,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.8538</v>
+        <v>5.9907</v>
       </c>
       <c r="C6">
-        <v>29.3091</v>
+        <v>74.3045</v>
       </c>
       <c r="D6">
-        <v>5.4138</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="E6">
-        <v>0.9554</v>
+        <v>0.8973</v>
       </c>
       <c r="F6">
-        <v>0.1047</v>
+        <v>0.1923</v>
       </c>
       <c r="G6">
-        <v>0.07480000000000001</v>
+        <v>0.138</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2347,22 +2347,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5984</v>
+        <v>4.4177</v>
       </c>
       <c r="C7">
-        <v>38.9276</v>
+        <v>37.7294</v>
       </c>
       <c r="D7">
-        <v>6.1874</v>
+        <v>5.9804</v>
       </c>
       <c r="E7">
-        <v>0.9486</v>
+        <v>0.9481000000000001</v>
       </c>
       <c r="F7">
-        <v>0.1129</v>
+        <v>0.1072</v>
       </c>
       <c r="G7">
-        <v>0.08649999999999999</v>
+        <v>0.08260000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2370,22 +2370,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.5387999999999999</v>
+        <v>0.8028</v>
       </c>
       <c r="C8">
-        <v>10.0889</v>
+        <v>18.9024</v>
       </c>
       <c r="D8">
-        <v>0.8024</v>
+        <v>1.4015</v>
       </c>
       <c r="E8">
-        <v>0.01</v>
+        <v>0.0272</v>
       </c>
       <c r="F8">
-        <v>0.0343</v>
+        <v>0.0427</v>
       </c>
       <c r="G8">
-        <v>0.0234</v>
+        <v>0.0278</v>
       </c>
     </row>
   </sheetData>
@@ -2429,22 +2429,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.9086</v>
+        <v>4.1226</v>
       </c>
       <c r="C2">
-        <v>23.294</v>
+        <v>30.4044</v>
       </c>
       <c r="D2">
-        <v>4.8264</v>
+        <v>5.514</v>
       </c>
       <c r="E2">
-        <v>0.9717</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="F2">
-        <v>0.0643</v>
+        <v>0.09379999999999999</v>
       </c>
       <c r="G2">
-        <v>0.0563</v>
+        <v>0.06950000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2452,22 +2452,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.3399</v>
+        <v>4.0592</v>
       </c>
       <c r="C3">
-        <v>61.0785</v>
+        <v>27.9588</v>
       </c>
       <c r="D3">
-        <v>7.8153</v>
+        <v>5.2876</v>
       </c>
       <c r="E3">
-        <v>0.9137999999999999</v>
+        <v>0.9658</v>
       </c>
       <c r="F3">
-        <v>0.1114</v>
+        <v>0.0885</v>
       </c>
       <c r="G3">
-        <v>0.0851</v>
+        <v>0.0702</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2475,22 +2475,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.1576</v>
+        <v>4.2494</v>
       </c>
       <c r="C4">
-        <v>26.6576</v>
+        <v>32.5908</v>
       </c>
       <c r="D4">
-        <v>5.1631</v>
+        <v>5.7088</v>
       </c>
       <c r="E4">
-        <v>0.9597</v>
+        <v>0.9482</v>
       </c>
       <c r="F4">
-        <v>0.09030000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="G4">
-        <v>0.07290000000000001</v>
+        <v>0.0708</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2498,22 +2498,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.7948</v>
+        <v>3.1466</v>
       </c>
       <c r="C5">
-        <v>61.4996</v>
+        <v>16.0764</v>
       </c>
       <c r="D5">
-        <v>7.8422</v>
+        <v>4.0095</v>
       </c>
       <c r="E5">
-        <v>0.9326</v>
+        <v>0.9805</v>
       </c>
       <c r="F5">
-        <v>0.1865</v>
+        <v>0.07580000000000001</v>
       </c>
       <c r="G5">
-        <v>0.138</v>
+        <v>0.0582</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2521,22 +2521,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.7863</v>
+        <v>6.0815</v>
       </c>
       <c r="C6">
-        <v>26.4179</v>
+        <v>79.57170000000001</v>
       </c>
       <c r="D6">
-        <v>5.1398</v>
+        <v>8.920299999999999</v>
       </c>
       <c r="E6">
-        <v>0.9598</v>
+        <v>0.8901</v>
       </c>
       <c r="F6">
-        <v>0.1006</v>
+        <v>0.1887</v>
       </c>
       <c r="G6">
-        <v>0.0716</v>
+        <v>0.1348</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2544,22 +2544,22 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>4.5974</v>
+        <v>4.3319</v>
       </c>
       <c r="C7">
-        <v>39.7895</v>
+        <v>37.3204</v>
       </c>
       <c r="D7">
-        <v>6.1574</v>
+        <v>5.8881</v>
       </c>
       <c r="E7">
-        <v>0.9475</v>
+        <v>0.9486</v>
       </c>
       <c r="F7">
-        <v>0.1106</v>
+        <v>0.1074</v>
       </c>
       <c r="G7">
-        <v>0.0848</v>
+        <v>0.08069999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2567,22 +2567,22 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>0.8137</v>
+        <v>0.9582000000000001</v>
       </c>
       <c r="C8">
-        <v>17.5949</v>
+        <v>21.883</v>
       </c>
       <c r="D8">
-        <v>1.3699</v>
+        <v>1.6282</v>
       </c>
       <c r="E8">
-        <v>0.0212</v>
+        <v>0.0311</v>
       </c>
       <c r="F8">
-        <v>0.041</v>
+        <v>0.0411</v>
       </c>
       <c r="G8">
-        <v>0.0281</v>
+        <v>0.0274</v>
       </c>
     </row>
   </sheetData>
@@ -2629,22 +2629,22 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>4.5871</v>
+        <v>4.4767</v>
       </c>
       <c r="D2">
-        <v>34.2862</v>
+        <v>29.2559</v>
       </c>
       <c r="E2">
-        <v>5.8554</v>
+        <v>5.4089</v>
       </c>
       <c r="F2">
-        <v>0.9308</v>
+        <v>0.9404</v>
       </c>
       <c r="G2">
-        <v>0.093</v>
+        <v>0.08890000000000001</v>
       </c>
       <c r="H2">
-        <v>0.07729999999999999</v>
+        <v>0.0751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>